<commit_message>
gerber files for v2-1 w J1 update
</commit_message>
<xml_diff>
--- a/designs/Pufferfish-Interface-2/reference/Interface Bill of Materials v2-1.xlsx
+++ b/designs/Pufferfish-Interface-2/reference/Interface Bill of Materials v2-1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurenadachi/Documents/GitHub/pufferfish-electronics/designs/Pufferfish-Interface-2/reference/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C90483CE-6158-0D41-9F1A-952F236FF4FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA51433D-C54E-724A-B575-FB6EE7991C23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="460" windowWidth="25040" windowHeight="14040" xr2:uid="{AB4FADCF-5D3E-0F4F-A6DE-656B770204FC}"/>
+    <workbookView xWindow="1860" yWindow="460" windowWidth="25040" windowHeight="14040" xr2:uid="{AB4FADCF-5D3E-0F4F-A6DE-656B770204FC}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM Interface" sheetId="3" r:id="rId1"/>
@@ -1479,8 +1479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E9B5640-6FAA-8446-9BE8-A4CA60B8E992}">
   <dimension ref="A1:P30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="114" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" zoomScale="114" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
before adding the microphone
</commit_message>
<xml_diff>
--- a/designs/Pufferfish-Interface-2/reference/Interface Bill of Materials v2-1.xlsx
+++ b/designs/Pufferfish-Interface-2/reference/Interface Bill of Materials v2-1.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurenadachi/Documents/GitHub/pufferfish-electronics/designs/Pufferfish-Interface-2/reference/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA51433D-C54E-724A-B575-FB6EE7991C23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{708F4E36-D1B3-2041-8E1F-518043CFA3A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="460" windowWidth="25040" windowHeight="14040" xr2:uid="{AB4FADCF-5D3E-0F4F-A6DE-656B770204FC}"/>
+    <workbookView xWindow="8260" yWindow="460" windowWidth="25040" windowHeight="14040" activeTab="2" xr2:uid="{AB4FADCF-5D3E-0F4F-A6DE-656B770204FC}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM Interface" sheetId="3" r:id="rId1"/>
     <sheet name="BOM Pi" sheetId="4" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
-    <sheet name="Digikey order" sheetId="2" r:id="rId4"/>
+    <sheet name="BOM Interface 2-2" sheetId="5" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Digikey order" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="278">
   <si>
     <t>ID</t>
   </si>
@@ -750,13 +751,133 @@
   </si>
   <si>
     <t>https://www.digikey.com/product-detail/en/molex/0022272091/WM4118-ND/1130584</t>
+  </si>
+  <si>
+    <t>Contol board to Pi</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/TE-Connectivity/1-1658527-3?qs=3csLVnQQLU2jT%252BbogjRSzQ%3D%3D</t>
+  </si>
+  <si>
+    <t>1-1658527-3</t>
+  </si>
+  <si>
+    <t>571-1-1658527-3</t>
+  </si>
+  <si>
+    <t>Digikey search: https://www.mouser.com/Connectors/Headers-Wire-Housings/_/N-ay0lo?P=1ytkn6hZ1ytkn06Z1z0wxp6&amp;Keyword=female+connector&amp;FS=True</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>SB6286</t>
+  </si>
+  <si>
+    <t>Mic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TL072CDT </t>
+  </si>
+  <si>
+    <t>D3,4</t>
+  </si>
+  <si>
+    <t>1N4148WT</t>
+  </si>
+  <si>
+    <t>If we want SPI insead of ADC out</t>
+  </si>
+  <si>
+    <t>U3A,B,P</t>
+  </si>
+  <si>
+    <t>﻿SMA</t>
+  </si>
+  <si>
+    <t>﻿SO08</t>
+  </si>
+  <si>
+    <t>﻿SO08-EIAJ_MCU</t>
+  </si>
+  <si>
+    <t>﻿SOT23-6</t>
+  </si>
+  <si>
+    <t>﻿SOD523</t>
+  </si>
+  <si>
+    <t>﻿MIC2-D9.7XH4.5MM</t>
+  </si>
+  <si>
+    <t>https://lcsc.com/product-detail/DC-DC-Converters_SB6286_C157668.html</t>
+  </si>
+  <si>
+    <t>International</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/stmicroelectronics/TL072CDT/497-2200-1-ND/599107</t>
+  </si>
+  <si>
+    <t>8-SOIC</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/on-semiconductor/1N4148WT/1N4148WTCT-ND/2094398</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/STMicroelectronics/TL072CDT?qs=6fffrORWf5pLFxBvwrMMAA%3D%3D</t>
+  </si>
+  <si>
+    <t>Tiny85-20-SMT  (ATTINY85-20SU)</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/microchip-technology/ATTINY85-20SU/ATTINY85-20SU-ND/735470?utm_campaign=buynow&amp;utm_medium=aggregator&amp;WT.z_cid=ref_findchips_standard&amp;utm_source=findchips</t>
+  </si>
+  <si>
+    <t>SC-79, SOD-523F</t>
+  </si>
+  <si>
+    <t>(On eagle)</t>
+  </si>
+  <si>
+    <t>4.7 uH +-20%</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/taiyo-yuden/NRS5030T4R7MMGJV/587-3605-1-ND/4694114</t>
+  </si>
+  <si>
+    <t>Search: https://www.digikey.com/products/en/inductors-coils-chokes/fixed-inductors/71?FV=-8%7C71%2C3%7C1900%2C69%7C409393%2C80%7C402031%2C1989%7C0%2Cmu4.7µH%7C2087&amp;quantity=0&amp;ColumnSort=-1000009&amp;page=1&amp;k=inductor&amp;pageSize=25&amp;pkeyword=inductor</t>
+  </si>
+  <si>
+    <t>More options</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/on-semiconductor/SS22T3G/SS22T3GOSCT-ND/4331834</t>
+  </si>
+  <si>
+    <t>SS22T3G</t>
+  </si>
+  <si>
+    <t>DO-214AA, SMB</t>
+  </si>
+  <si>
+    <t>SOT-23-6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">﻿L4030, PRS4018-4R7MT </t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/samsung-electro-mechanics/CIGW252010EH4R7MNE/1276-6931-1-ND/7041331</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="37" x14ac:knownFonts="1">
+  <fonts count="43" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1018,6 +1139,43 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF4F4F4F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF444444"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -1070,7 +1228,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
@@ -1162,6 +1320,13 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="38" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="42" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1479,7 +1644,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E9B5640-6FAA-8446-9BE8-A4CA60B8E992}">
   <dimension ref="A1:P30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="114" workbookViewId="0">
+    <sheetView zoomScale="114" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -2261,20 +2426,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B81DA78-FD1B-474D-AB22-5A2533BD4F55}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A2" sqref="A2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="66" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2299,7 +2464,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>201</v>
       </c>
@@ -2326,7 +2491,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>199</v>
       </c>
@@ -2349,7 +2514,7 @@
       <c r="H4" s="9"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>197</v>
       </c>
@@ -2370,7 +2535,7 @@
       <c r="H5" s="9"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>195</v>
       </c>
@@ -2387,7 +2552,7 @@
       <c r="H6" s="9"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
@@ -2398,7 +2563,7 @@
       <c r="H7" s="9"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>67</v>
       </c>
@@ -2423,7 +2588,7 @@
       </c>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
         <v>197</v>
       </c>
@@ -2446,7 +2611,7 @@
       <c r="H9" s="9"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
         <v>198</v>
       </c>
@@ -2469,7 +2634,7 @@
       <c r="H10" s="9"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
         <v>195</v>
       </c>
@@ -2490,7 +2655,7 @@
       <c r="H11" s="9"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
         <v>195</v>
       </c>
@@ -2507,7 +2672,7 @@
       <c r="H12" s="9"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>196</v>
       </c>
@@ -2524,7 +2689,7 @@
       <c r="H13" s="9"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
         <v>196</v>
       </c>
@@ -2541,7 +2706,7 @@
       <c r="H14" s="9"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" ht="23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="23" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>197</v>
       </c>
@@ -2561,6 +2726,29 @@
       <c r="G15" s="9"/>
       <c r="H15" s="9"/>
       <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="B16" s="73" t="s">
+        <v>240</v>
+      </c>
+      <c r="C16" s="9">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>238</v>
+      </c>
+      <c r="E16" s="73" t="s">
+        <v>241</v>
+      </c>
+      <c r="F16" t="s">
+        <v>239</v>
+      </c>
+      <c r="O16" t="s">
+        <v>242</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2579,6 +2767,197 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAC86840-D8AD-F542-98B2-FC57B25AE1B6}">
+  <dimension ref="A1:J13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="10.83203125" style="74"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="74" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="74" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="74" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="74" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="74" t="s">
+        <v>78</v>
+      </c>
+      <c r="F1" s="74" t="s">
+        <v>119</v>
+      </c>
+      <c r="G1" s="74" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="74" t="s">
+        <v>267</v>
+      </c>
+      <c r="J1" s="74" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="78" t="s">
+        <v>243</v>
+      </c>
+      <c r="B2" s="78" t="s">
+        <v>269</v>
+      </c>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78" t="s">
+        <v>268</v>
+      </c>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78" t="s">
+        <v>276</v>
+      </c>
+      <c r="I2" s="78" t="s">
+        <v>270</v>
+      </c>
+      <c r="J2" s="78" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="74" t="s">
+        <v>244</v>
+      </c>
+      <c r="B3" s="77" t="s">
+        <v>273</v>
+      </c>
+      <c r="F3" s="74" t="s">
+        <v>272</v>
+      </c>
+      <c r="G3" s="76" t="s">
+        <v>274</v>
+      </c>
+      <c r="H3" s="74" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="20" x14ac:dyDescent="0.2">
+      <c r="A4" s="78" t="s">
+        <v>136</v>
+      </c>
+      <c r="B4" s="78" t="s">
+        <v>245</v>
+      </c>
+      <c r="C4" s="78">
+        <v>1</v>
+      </c>
+      <c r="D4" s="78"/>
+      <c r="E4" s="78"/>
+      <c r="F4" s="78" t="s">
+        <v>258</v>
+      </c>
+      <c r="G4" s="79" t="s">
+        <v>275</v>
+      </c>
+      <c r="H4" s="78" t="s">
+        <v>255</v>
+      </c>
+      <c r="I4" s="74" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="78" t="s">
+        <v>246</v>
+      </c>
+      <c r="B5" s="78"/>
+      <c r="C5" s="78"/>
+      <c r="D5" s="78"/>
+      <c r="E5" s="78"/>
+      <c r="F5" s="78"/>
+      <c r="G5" s="78"/>
+      <c r="H5" s="78" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="74" t="s">
+        <v>251</v>
+      </c>
+      <c r="B6" s="75" t="s">
+        <v>247</v>
+      </c>
+      <c r="F6" s="74" t="s">
+        <v>260</v>
+      </c>
+      <c r="G6" s="74" t="s">
+        <v>261</v>
+      </c>
+      <c r="H6" s="74" t="s">
+        <v>253</v>
+      </c>
+      <c r="J6" s="74" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="74" t="s">
+        <v>248</v>
+      </c>
+      <c r="B7" s="74" t="s">
+        <v>249</v>
+      </c>
+      <c r="F7" s="74" t="s">
+        <v>262</v>
+      </c>
+      <c r="G7" s="76" t="s">
+        <v>266</v>
+      </c>
+      <c r="H7" s="74" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B8" s="75" t="s">
+        <v>264</v>
+      </c>
+      <c r="D8" s="74" t="s">
+        <v>250</v>
+      </c>
+      <c r="F8" s="74" t="s">
+        <v>265</v>
+      </c>
+      <c r="G8" s="76" t="s">
+        <v>261</v>
+      </c>
+      <c r="H8" s="74" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="74" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="74" t="s">
+        <v>196</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB09F318-339D-2C4D-BE3F-E973DAF25A4A}">
   <dimension ref="A1:R41"/>
   <sheetViews>
@@ -3449,7 +3828,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E531EC0F-8B5B-B945-81ED-74853B083270}">
   <dimension ref="A1:R41"/>
   <sheetViews>

</xml_diff>

<commit_message>
add buzzer and started accomodating 6 buttons
</commit_message>
<xml_diff>
--- a/designs/Pufferfish-Interface-2/reference/Interface Bill of Materials v2-1.xlsx
+++ b/designs/Pufferfish-Interface-2/reference/Interface Bill of Materials v2-1.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurenadachi/Documents/GitHub/pufferfish-electronics/designs/Pufferfish-Interface-2/reference/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F7EEF6-1E02-544A-A897-E06063715979}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F24E66C-55C0-8E4E-A585-A2734672D1F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-380" yWindow="460" windowWidth="25040" windowHeight="14040" activeTab="2" xr2:uid="{AB4FADCF-5D3E-0F4F-A6DE-656B770204FC}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="25040" windowHeight="14040" xr2:uid="{AB4FADCF-5D3E-0F4F-A6DE-656B770204FC}"/>
   </bookViews>
   <sheets>
-    <sheet name="BOM Interface" sheetId="3" r:id="rId1"/>
-    <sheet name="BOM Pi" sheetId="4" r:id="rId2"/>
-    <sheet name="BOM Interface 2-2" sheetId="5" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
-    <sheet name="Digikey order" sheetId="2" r:id="rId5"/>
+    <sheet name="BOM Interface 2-3" sheetId="6" r:id="rId1"/>
+    <sheet name="BOM Interface" sheetId="3" r:id="rId2"/>
+    <sheet name="BOM Pi" sheetId="4" r:id="rId3"/>
+    <sheet name="BOM Interface 2-2" sheetId="5" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId5"/>
+    <sheet name="Digikey order" sheetId="2" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="308">
   <si>
     <t>ID</t>
   </si>
@@ -880,13 +881,179 @@
   </si>
   <si>
     <t>Package_SO SOIC-8_3.9x4.9mm_P1.27mm</t>
+  </si>
+  <si>
+    <t>https://statics3.seeedstudio.com/images/opl/datasheet/312030029.pdf</t>
+  </si>
+  <si>
+    <r>
+      <t>-40±3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">dB </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Φ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman,Bold"/>
+      </rPr>
+      <t>9.7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>±</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman,Bold"/>
+      </rPr>
+      <t>0.1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman,Bold"/>
+      </rPr>
+      <t>4.5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>±</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman,Bold"/>
+      </rPr>
+      <t xml:space="preserve">0.2(H)mm </t>
+    </r>
+  </si>
+  <si>
+    <t>Sensitivity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Omni-directional </t>
+  </si>
+  <si>
+    <t>Operating impedance</t>
+  </si>
+  <si>
+    <r>
+      <t>2.2K</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial,Bold"/>
+      </rPr>
+      <t xml:space="preserve">Ω </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Standard Power Supply </t>
+  </si>
+  <si>
+    <t>2V</t>
+  </si>
+  <si>
+    <t>Operating voltage</t>
+  </si>
+  <si>
+    <t>Freq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50-16,000Hz </t>
+  </si>
+  <si>
+    <t>Current consumption</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M ax.0.5mA </t>
+  </si>
+  <si>
+    <t>S/N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">More than 58dB </t>
+  </si>
+  <si>
+    <t>D.C 1-10V</t>
+  </si>
+  <si>
+    <t>Search for similar: https://www.digikey.com/products/en/audio-products/microphones/158?k=microphone&amp;k=&amp;pkeyword=microphone&amp;sv=0&amp;pv54=225814&amp;pv54=224446&amp;pv54=431168&amp;pv54=220285&amp;pv54=219087&amp;pv54=217857&amp;pv54=217859&amp;pv54=214660&amp;sf=1&amp;FV=1989%7C0%2C-8%7C158%2C231%7C246852%2C231%7C247605%2C231%7C257128%2C231%7C258336%2C231%7C258607%2C231%7C259500%2C231%7C260531%2C231%7C260825%2C231%7C260870%2C231%7C261458%2C231%7C262804%2C231%7C263258%2C231%7C263807%2C231%7C264516%2C231%7C265253%2C231%7C266159%2C231%7C273661%2C231%7C275473%2C231%7C276822%2C231%7C279349%2C231%7C287126%2C630%7C381840%2Cmu2V%7C2079%2Cyr1V+%7E+10V%7C2142%2Cyr100Hz+%7E+10kHz%7C2145%2Cyr100Hz+%7E+12kHz%7C2145%2Cyr100Hz+%7E+15kHz%7C2145%2Cyr100Hz+%7E+16kHz%7C2145%2Cyr100Hz+%7E+20kHz%7C2145%2Cyr100Hz+%7E+4.8kHz%7C2145%2Cyr100Hz+%7E+4kHz%7C2145%2Cyr100Hz+%7E+5.5kHz%7C2145%2Cyr100Hz+%7E+5.8kHz%7C2145%2Cyr100Hz+%7E+5kHz%7C2145%2Cyr100Hz+%7E+6kHz%7C2145%2Cyr100Hz+%7E+80kHz%7C2145%2Cyr100Hz+%7E+8kHz%7C2145%2Cyr10Hz+%7E+10kHz%7C2145%2Cyr15Hz+%7E+16kHz%7C2145%2Cyr20Hz+%7E+10kHz%7C2145%2Cyr20Hz+%7E+15kHz%7C2145%2Cyr20Hz+%7E+16kHz%7C2145%2Cyr20Hz+%7E+18kHz%7C2145%2Cyr20Hz+%7E+20kHz%7C2145%2Cyr20Hz+%7E+8kHz%7C2145%2Cyr25Hz+%7E+20kHz%7C2145%2Cyr30Hz+%7E+10kHz%7C2145%2Cyr30Hz+%7E+15kHz%7C2145%2Cyr35Hz+%7E+20kHz%7C2145%2Cyr45Hz+%7E+20kHz%7C2145%2Cyr50Hz+%7E+10kHz%7C2145%2Cyr50Hz+%7E+12kHz%7C2145%2Cyr50Hz+%7E+16kHz%7C2145%2Cyr50Hz+%7E+20kHz%7C2145%2Cyr50Hz+%7E+40kHz%7C2145%2Cyr50Hz+%7E+80kHz%7C2145%2Cyr60Hz+%7E+20kHz%7C2145%2Cyr6Hz+%7E+20kHz%7C2145%2Cyr77Hz+%7E+20kHz%7C2145%2Cyr80Hz+%7E+10kHz%7C2145%2Cyr80Hz+%7E+20kHz%7C2145%2Cyr90Hz+%7E+16kHz%7C2145&amp;quantity=&amp;ColumnSort=-1000009&amp;page=1&amp;stock=1&amp;pageSize=25</t>
+  </si>
+  <si>
+    <t>Similar options</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/soberton-inc/EM-6050P/433-1093-ND/3973685</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/soberton-inc/EM-6022P/433-1088-ND/3973680</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/cui-devices/CSQG703BP/102-1286-ND/671242</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BUZZ2 </t>
+  </si>
+  <si>
+    <t>CSQG703BP</t>
+  </si>
+  <si>
+    <t>5103308-5</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/te-connectivity-amp-connectors/5103308-5/A33165-ND/1114903</t>
+  </si>
+  <si>
+    <t>A33165-ND</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="45" x14ac:knownFonts="1">
+  <fonts count="53">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1197,6 +1364,52 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial,Bold"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman,Bold"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman,Bold"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial,Bold"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -1255,7 +1468,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
@@ -1362,6 +1575,13 @@
     <xf numFmtId="0" fontId="41" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="43" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1676,14 +1896,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E9B5640-6FAA-8446-9BE8-A4CA60B8E992}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85374FF2-138F-FD4F-BB74-E6C88CA0C0BE}">
   <dimension ref="A1:P30"/>
   <sheetViews>
-    <sheetView zoomScale="114" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" zoomScale="114" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="2" width="10.83203125" style="1"/>
     <col min="3" max="3" width="16.33203125" style="1" customWidth="1"/>
@@ -1698,7 +1918,7 @@
     <col min="12" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>225</v>
       </c>
@@ -1736,7 +1956,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13">
       <c r="A2" s="55" t="s">
         <v>212</v>
       </c>
@@ -1768,7 +1988,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13">
       <c r="A3" s="55" t="s">
         <v>213</v>
       </c>
@@ -1797,28 +2017,29 @@
         <v>452000</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="55" t="s">
+    <row r="4" spans="1:13">
+      <c r="A4" s="93" t="s">
         <v>214</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="2">
-        <v>1</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="C4" s="48" t="s">
+        <v>305</v>
+      </c>
+      <c r="D4" s="94">
+        <v>1</v>
+      </c>
+      <c r="E4" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>25</v>
-      </c>
+      <c r="F4" s="48" t="s">
+        <v>307</v>
+      </c>
+      <c r="G4" s="49" t="s">
+        <v>306</v>
+      </c>
+      <c r="H4" s="48"/>
       <c r="J4" s="16">
         <v>2500</v>
       </c>
@@ -1826,7 +2047,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13">
       <c r="A5" s="55" t="s">
         <v>215</v>
       </c>
@@ -1855,7 +2076,7 @@
         <v>49000</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13">
       <c r="A6" s="55" t="s">
         <v>216</v>
       </c>
@@ -1893,7 +2114,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13">
       <c r="A7" s="55" t="s">
         <v>217</v>
       </c>
@@ -1925,7 +2146,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13">
       <c r="A8" s="55" t="s">
         <v>218</v>
       </c>
@@ -1951,7 +2172,7 @@
         <v>42000</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13">
       <c r="A9" s="55" t="s">
         <v>219</v>
       </c>
@@ -1980,7 +2201,7 @@
         <v>75000</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13">
       <c r="A10" s="55" t="s">
         <v>220</v>
       </c>
@@ -2004,7 +2225,7 @@
       </c>
       <c r="J10" s="16"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13">
       <c r="A11" s="55" t="s">
         <v>221</v>
       </c>
@@ -2033,7 +2254,779 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="12" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" s="9" customFormat="1">
+      <c r="A12" s="55" t="s">
+        <v>222</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="9">
+        <f>10+6+8</f>
+        <v>24</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="H12" s="65"/>
+      <c r="I12" s="60"/>
+      <c r="J12" s="16"/>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="55" t="s">
+        <v>223</v>
+      </c>
+      <c r="B13" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="C13" s="72">
+        <v>1718560009</v>
+      </c>
+      <c r="D13" s="26">
+        <v>1</v>
+      </c>
+      <c r="E13" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="F13" s="21" t="s">
+        <v>236</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="I13" s="9"/>
+      <c r="J13" s="16">
+        <v>20390000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" s="38" customFormat="1">
+      <c r="A14" s="55" t="s">
+        <v>224</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D14" s="9">
+        <v>1</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="F14" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="H14" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="I14" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="J14" s="59">
+        <v>4000</v>
+      </c>
+      <c r="K14" s="38">
+        <v>15</v>
+      </c>
+      <c r="L14" s="38" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="B15" s="48" t="s">
+        <v>303</v>
+      </c>
+      <c r="C15" s="41" t="s">
+        <v>304</v>
+      </c>
+      <c r="D15" s="48">
+        <v>1</v>
+      </c>
+      <c r="E15" s="44"/>
+      <c r="F15" s="48"/>
+      <c r="G15" s="49" t="s">
+        <v>302</v>
+      </c>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="16">
+        <v>4500</v>
+      </c>
+      <c r="K15" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
+      <c r="P17" s="29"/>
+    </row>
+    <row r="18" spans="1:16">
+      <c r="A18" s="55" t="s">
+        <v>226</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="D18" s="2">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F18" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="I18" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="J18" s="30" t="s">
+        <v>152</v>
+      </c>
+      <c r="P18" s="18"/>
+    </row>
+    <row r="19" spans="1:16">
+      <c r="A19" s="55" t="s">
+        <v>227</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="D19" s="1">
+        <v>4</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F19" s="21" t="s">
+        <v>168</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
+      <c r="A20" s="55" t="s">
+        <v>228</v>
+      </c>
+      <c r="B20" s="26" t="s">
+        <v>133</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="H20" s="3"/>
+      <c r="J20" s="16">
+        <v>35000</v>
+      </c>
+      <c r="K20" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16">
+      <c r="A21" s="55" t="s">
+        <v>229</v>
+      </c>
+      <c r="B21" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F21" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="J21" s="16"/>
+      <c r="P21" s="18"/>
+    </row>
+    <row r="22" spans="1:16">
+      <c r="A22" s="55" t="s">
+        <v>230</v>
+      </c>
+      <c r="B22" s="31" t="s">
+        <v>113</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D22" s="32">
+        <v>1</v>
+      </c>
+      <c r="E22" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="F22" s="32" t="s">
+        <v>161</v>
+      </c>
+      <c r="G22" s="58" t="s">
+        <v>76</v>
+      </c>
+      <c r="H22" s="32"/>
+      <c r="I22" s="34"/>
+      <c r="J22" s="17">
+        <v>60</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
+      <c r="A23" s="55" t="s">
+        <v>231</v>
+      </c>
+      <c r="B23" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="C23" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="F23" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="J23" s="17">
+        <v>0</v>
+      </c>
+      <c r="K23" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
+      <c r="A24" s="55" t="s">
+        <v>232</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C24" s="22" t="s">
+        <v>171</v>
+      </c>
+      <c r="D24" s="1">
+        <v>3</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="F24" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
+      <c r="A25" s="55" t="s">
+        <v>233</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D25" s="1">
+        <v>1</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="J25" s="16">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16">
+      <c r="B26" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D26" s="9">
+        <v>1</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="F26" s="9"/>
+      <c r="G26" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="H26" s="8"/>
+    </row>
+    <row r="27" spans="1:16" ht="13" customHeight="1">
+      <c r="B27" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="D27" s="1">
+        <v>1</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F27" s="15"/>
+      <c r="G27" s="6"/>
+      <c r="J27" s="19">
+        <v>758</v>
+      </c>
+      <c r="K27" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="L27" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16">
+      <c r="K30" s="1">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G9" r:id="rId1" display="https://www.digikey.com/product-detail/en/vishay-siliconix/2N7002E-T1-E3/2N7002E-T1-E3CT-ND/3946142?utm_adgroup=Semiconductor%20Modules&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Dynamic%20Search_RLSA_Buyers&amp;utm_term=&amp;utm_content=Semiconductor%20Modules&amp;gclid=Cj0KCQjwrIf3BRD1ARIsAMuugNtAYg0B4uzN6uG3FDVYlywiEKFAGbXRLO8hnfXG_d9twvCOg1_5j4waAs4CEALw_wcB" xr:uid="{78A24A15-31CF-9F47-A91F-FA441EF9C614}"/>
+    <hyperlink ref="G12" r:id="rId2" xr:uid="{73D98201-D87A-4B4B-A02A-29A5FAECD42E}"/>
+    <hyperlink ref="G20" r:id="rId3" xr:uid="{8CA4D74E-E935-2F42-93CC-3425476EDB88}"/>
+    <hyperlink ref="G3" r:id="rId4" xr:uid="{8791FA06-E3A4-1943-BFDF-87D3983EC694}"/>
+    <hyperlink ref="G5" r:id="rId5" xr:uid="{03BF4570-C52E-B244-9F90-52764ADFD1C5}"/>
+    <hyperlink ref="G8" r:id="rId6" xr:uid="{F9C832B3-42F8-D744-BBC6-D42227150E36}"/>
+    <hyperlink ref="G21" r:id="rId7" xr:uid="{F139212D-3876-314E-B9A8-32A838323003}"/>
+    <hyperlink ref="G6" r:id="rId8" xr:uid="{65E48627-1237-5243-A5A5-4DF4CF98D5E0}"/>
+    <hyperlink ref="G11" r:id="rId9" xr:uid="{51797C28-FED1-D443-9104-7306ACDF3AA3}"/>
+    <hyperlink ref="G14" r:id="rId10" xr:uid="{6AB19274-16AE-1F47-AA50-8E6B56033E01}"/>
+    <hyperlink ref="G25" r:id="rId11" xr:uid="{D37BCA5F-7D02-BC43-A9AF-97299644271B}"/>
+    <hyperlink ref="H23" r:id="rId12" xr:uid="{643D5EB8-96B1-8349-86E7-1106B7EEF44C}"/>
+    <hyperlink ref="G22" r:id="rId13" xr:uid="{3A799947-BEBC-EC4A-A0FF-D641DB274EDC}"/>
+    <hyperlink ref="G18" r:id="rId14" xr:uid="{D165C778-190D-4F4B-B93F-7CC39E60CF2D}"/>
+    <hyperlink ref="G7" r:id="rId15" xr:uid="{51412221-95CC-D040-BC45-2DF7E8EE65D6}"/>
+    <hyperlink ref="G10" r:id="rId16" display="https://www.digikey.com/product-detail/en/on-semiconductor/FDN337N/FDN337NCT-ND/458950?utm_adgroup=Semiconductor%20Modules&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Dynamic%20Search&amp;utm_term=&amp;utm_content=Semiconductor%20Modules&amp;gclid=EAIaIQobChMIi9eQ5_aJ6wIViZWzCh0mJgM4EAAYAyAAEgLjm_D_BwE" xr:uid="{4E70B157-27AD-0C43-B73B-B0A96F65C0B1}"/>
+    <hyperlink ref="G19" r:id="rId17" xr:uid="{CEF247F0-AC52-E148-9F68-14BD6BB6B45E}"/>
+    <hyperlink ref="G24" r:id="rId18" xr:uid="{01250BBC-38BA-5A4D-B165-4926E5F33703}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E9B5640-6FAA-8446-9BE8-A4CA60B8E992}">
+  <dimension ref="A1:P30"/>
+  <sheetViews>
+    <sheetView zoomScale="114" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
+  <cols>
+    <col min="1" max="2" width="10.83203125" style="1"/>
+    <col min="3" max="3" width="16.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="1"/>
+    <col min="7" max="7" width="42.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" style="1"/>
+    <col min="9" max="9" width="33.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="55" t="s">
+        <v>212</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>209</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="J2" s="27">
+        <v>560</v>
+      </c>
+      <c r="K2" s="1">
+        <v>4</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="55" t="s">
+        <v>213</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2">
+        <v>5</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="16">
+        <v>452000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="55" t="s">
+        <v>214</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="16">
+        <v>2500</v>
+      </c>
+      <c r="K4" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="55" t="s">
+        <v>215</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="16">
+        <v>49000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="55" t="s">
+        <v>216</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="17">
+        <v>684</v>
+      </c>
+      <c r="K6" s="1">
+        <v>16</v>
+      </c>
+      <c r="L6" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="55" t="s">
+        <v>217</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J7" s="16">
+        <v>17500</v>
+      </c>
+      <c r="K7" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="55" t="s">
+        <v>218</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="2">
+        <v>5</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="J8" s="16">
+        <v>42000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="55" t="s">
+        <v>219</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="2">
+        <v>7</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="J9" s="16">
+        <v>75000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="55" t="s">
+        <v>220</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>177</v>
+      </c>
+      <c r="D10" s="2">
+        <v>3</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" s="21" t="s">
+        <v>176</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="J10" s="16"/>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="55" t="s">
+        <v>221</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="D11" s="9">
+        <f>4</f>
+        <v>4</v>
+      </c>
+      <c r="E11" s="11">
+        <v>82</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="16">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" s="9" customFormat="1">
       <c r="A12" s="15"/>
       <c r="B12" s="60"/>
       <c r="C12" s="61" t="s">
@@ -2055,7 +3048,7 @@
       <c r="I12" s="60"/>
       <c r="J12" s="16"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13">
       <c r="A13" s="55" t="s">
         <v>222</v>
       </c>
@@ -2084,7 +3077,7 @@
         <v>20390000</v>
       </c>
     </row>
-    <row r="14" spans="1:13" s="38" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" s="38" customFormat="1">
       <c r="A14" s="55" t="s">
         <v>223</v>
       </c>
@@ -2122,7 +3115,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13">
       <c r="A15" s="55" t="s">
         <v>224</v>
       </c>
@@ -2153,7 +3146,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16">
       <c r="B17" s="13" t="s">
         <v>52</v>
       </c>
@@ -2162,7 +3155,7 @@
       <c r="G17" s="4"/>
       <c r="P17" s="29"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16">
       <c r="A18" s="55" t="s">
         <v>226</v>
       </c>
@@ -2192,7 +3185,7 @@
       </c>
       <c r="P18" s="18"/>
     </row>
-    <row r="19" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" ht="16">
       <c r="A19" s="55" t="s">
         <v>227</v>
       </c>
@@ -2218,7 +3211,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16">
       <c r="A20" s="55" t="s">
         <v>228</v>
       </c>
@@ -2248,7 +3241,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16">
       <c r="A21" s="55" t="s">
         <v>229</v>
       </c>
@@ -2276,7 +3269,7 @@
       <c r="J21" s="16"/>
       <c r="P21" s="18"/>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16">
       <c r="A22" s="55" t="s">
         <v>230</v>
       </c>
@@ -2307,7 +3300,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16">
       <c r="A23" s="55" t="s">
         <v>231</v>
       </c>
@@ -2333,7 +3326,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" ht="16">
       <c r="A24" s="55" t="s">
         <v>232</v>
       </c>
@@ -2356,7 +3349,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16">
       <c r="A25" s="55" t="s">
         <v>233</v>
       </c>
@@ -2382,7 +3375,7 @@
         <v>7500</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16">
       <c r="B26" s="1" t="s">
         <v>166</v>
       </c>
@@ -2398,7 +3391,7 @@
       </c>
       <c r="H26" s="8"/>
     </row>
-    <row r="27" spans="1:16" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" ht="13" customHeight="1">
       <c r="B27" s="1" t="s">
         <v>134</v>
       </c>
@@ -2426,7 +3419,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16">
       <c r="K30" s="1">
         <v>8</v>
       </c>
@@ -2459,7 +3452,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B81DA78-FD1B-474D-AB22-5A2533BD4F55}">
   <dimension ref="A1:O16"/>
   <sheetViews>
@@ -2467,14 +3460,14 @@
       <selection activeCell="A2" sqref="A2:G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15">
       <c r="A1" s="66" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2499,7 +3492,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15">
       <c r="A3" s="9" t="s">
         <v>201</v>
       </c>
@@ -2526,7 +3519,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15">
       <c r="A4" s="9" t="s">
         <v>199</v>
       </c>
@@ -2549,7 +3542,7 @@
       <c r="H4" s="9"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15">
       <c r="A5" s="9" t="s">
         <v>197</v>
       </c>
@@ -2570,7 +3563,7 @@
       <c r="H5" s="9"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15">
       <c r="A6" s="9" t="s">
         <v>195</v>
       </c>
@@ -2587,7 +3580,7 @@
       <c r="H6" s="9"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15">
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
@@ -2598,7 +3591,7 @@
       <c r="H7" s="9"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15">
       <c r="A8" s="9" t="s">
         <v>67</v>
       </c>
@@ -2623,7 +3616,7 @@
       </c>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15">
       <c r="A9" s="9" t="s">
         <v>197</v>
       </c>
@@ -2646,7 +3639,7 @@
       <c r="H9" s="9"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15">
       <c r="A10" s="9" t="s">
         <v>198</v>
       </c>
@@ -2669,7 +3662,7 @@
       <c r="H10" s="9"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15">
       <c r="A11" s="9" t="s">
         <v>195</v>
       </c>
@@ -2690,7 +3683,7 @@
       <c r="H11" s="9"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15">
       <c r="A12" s="9" t="s">
         <v>195</v>
       </c>
@@ -2707,7 +3700,7 @@
       <c r="H12" s="9"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15">
       <c r="A13" s="9" t="s">
         <v>196</v>
       </c>
@@ -2724,7 +3717,7 @@
       <c r="H13" s="9"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15">
       <c r="A14" s="9" t="s">
         <v>196</v>
       </c>
@@ -2741,7 +3734,7 @@
       <c r="H14" s="9"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:15" ht="23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="23">
       <c r="A15" s="9" t="s">
         <v>197</v>
       </c>
@@ -2762,7 +3755,7 @@
       <c r="H15" s="9"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" ht="17">
       <c r="A16" s="9" t="s">
         <v>197</v>
       </c>
@@ -2801,20 +3794,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAC86840-D8AD-F542-98B2-FC57B25AE1B6}">
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="16384" width="10.83203125" style="74"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12">
       <c r="A1" s="74" t="s">
         <v>0</v>
       </c>
@@ -2846,7 +3839,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12">
       <c r="A2" s="83" t="s">
         <v>243</v>
       </c>
@@ -2872,7 +3865,7 @@
       <c r="K2" s="84"/>
       <c r="L2" s="80"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12">
       <c r="A3" s="80" t="s">
         <v>244</v>
       </c>
@@ -2896,7 +3889,7 @@
       <c r="K3" s="80"/>
       <c r="L3" s="80"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12">
       <c r="A4" s="83" t="s">
         <v>136</v>
       </c>
@@ -2924,7 +3917,7 @@
       <c r="K4" s="85"/>
       <c r="L4" s="80"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12">
       <c r="A5" s="77" t="s">
         <v>246</v>
       </c>
@@ -2937,9 +3930,15 @@
       <c r="H5" s="77" t="s">
         <v>257</v>
       </c>
+      <c r="J5" s="74" t="s">
+        <v>281</v>
+      </c>
       <c r="K5" s="79"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L5" s="74" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" s="74" t="s">
         <v>251</v>
       </c>
@@ -2963,7 +3962,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12">
       <c r="A7" s="74" t="s">
         <v>248</v>
       </c>
@@ -2984,7 +3983,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12">
       <c r="B8" s="80" t="s">
         <v>264</v>
       </c>
@@ -3004,14 +4003,89 @@
       </c>
       <c r="I8" s="80"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12">
+      <c r="J11" s="74" t="s">
+        <v>284</v>
+      </c>
+      <c r="K11" s="88" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="19">
       <c r="A12" s="74" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K12" s="89" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="19">
       <c r="A13" s="74" t="s">
         <v>196</v>
+      </c>
+      <c r="K13" s="90" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="J14" s="74" t="s">
+        <v>286</v>
+      </c>
+      <c r="K14" s="91" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="J15" s="92" t="s">
+        <v>288</v>
+      </c>
+      <c r="K15" s="74" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="J16" s="74" t="s">
+        <v>290</v>
+      </c>
+      <c r="K16" s="92" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="17" spans="10:11">
+      <c r="J17" s="74" t="s">
+        <v>291</v>
+      </c>
+      <c r="K17" s="91" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="18" spans="10:11">
+      <c r="J18" s="74" t="s">
+        <v>293</v>
+      </c>
+      <c r="K18" s="91" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="19" spans="10:11">
+      <c r="J19" s="74" t="s">
+        <v>295</v>
+      </c>
+      <c r="K19" s="91" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="20" spans="10:11">
+      <c r="J20" s="74" t="s">
+        <v>299</v>
+      </c>
+      <c r="K20" s="74" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="21" spans="10:11">
+      <c r="K21" s="74" t="s">
+        <v>301</v>
       </c>
     </row>
   </sheetData>
@@ -3019,7 +4093,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB09F318-339D-2C4D-BE3F-E973DAF25A4A}">
   <dimension ref="A1:R41"/>
   <sheetViews>
@@ -3027,7 +4101,7 @@
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="1"/>
     <col min="2" max="2" width="16.33203125" style="1" customWidth="1"/>
@@ -3040,7 +4114,7 @@
     <col min="9" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3075,7 +4149,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -3104,7 +4178,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18">
       <c r="A3" s="1" t="s">
         <v>97</v>
       </c>
@@ -3130,7 +4204,7 @@
         <v>452000</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -3156,7 +4230,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
@@ -3182,7 +4256,7 @@
         <v>49000</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18">
       <c r="A6" s="1" t="s">
         <v>26</v>
       </c>
@@ -3217,7 +4291,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" ht="16">
       <c r="A7" s="1" t="s">
         <v>96</v>
       </c>
@@ -3246,7 +4320,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" ht="16">
       <c r="A8" s="1" t="s">
         <v>32</v>
       </c>
@@ -3269,7 +4343,7 @@
         <v>42000</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18">
       <c r="A9" s="1" t="s">
         <v>95</v>
       </c>
@@ -3295,7 +4369,7 @@
         <v>75000</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18">
       <c r="A10" s="1" t="s">
         <v>41</v>
       </c>
@@ -3321,7 +4395,7 @@
         <v>283000</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18">
       <c r="A11" s="9" t="s">
         <v>100</v>
       </c>
@@ -3347,7 +4421,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="12" spans="1:18" s="9" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" s="9" customFormat="1" ht="16">
       <c r="B12" s="54" t="s">
         <v>163</v>
       </c>
@@ -3366,7 +4440,7 @@
       <c r="G12" s="11"/>
       <c r="I12" s="16"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18">
       <c r="A13" s="9" t="s">
         <v>102</v>
       </c>
@@ -3394,7 +4468,7 @@
         <v>20390000</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18">
       <c r="A14" s="9" t="s">
         <v>82</v>
       </c>
@@ -3426,7 +4500,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18">
       <c r="B15" s="9" t="s">
         <v>87</v>
       </c>
@@ -3451,7 +4525,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18">
       <c r="A16" s="13" t="s">
         <v>52</v>
       </c>
@@ -3465,7 +4539,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17">
       <c r="A17" s="1" t="s">
         <v>136</v>
       </c>
@@ -3484,7 +4558,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" ht="16">
       <c r="A18" s="26" t="s">
         <v>51</v>
       </c>
@@ -3519,7 +4593,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17">
       <c r="A19" s="31" t="s">
         <v>113</v>
       </c>
@@ -3555,7 +4629,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="20" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" ht="16">
       <c r="A20" s="26" t="s">
         <v>114</v>
       </c>
@@ -3581,7 +4655,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" ht="16">
       <c r="B21" s="25" t="s">
         <v>129</v>
       </c>
@@ -3607,7 +4681,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17">
       <c r="A22" s="26" t="s">
         <v>132</v>
       </c>
@@ -3633,7 +4707,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17">
       <c r="A23" s="1" t="s">
         <v>133</v>
       </c>
@@ -3657,7 +4731,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17">
       <c r="A24" s="1" t="s">
         <v>134</v>
       </c>
@@ -3684,7 +4758,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:17">
       <c r="C25" s="9">
         <v>1</v>
       </c>
@@ -3696,7 +4770,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17">
       <c r="A26" s="13" t="s">
         <v>63</v>
       </c>
@@ -3704,7 +4778,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:17">
       <c r="A27" s="1" t="s">
         <v>68</v>
       </c>
@@ -3733,7 +4807,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:17">
       <c r="A28" s="9" t="s">
         <v>67</v>
       </c>
@@ -3760,15 +4834,15 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:17">
       <c r="I29" s="27"/>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:17">
       <c r="B30" s="9"/>
       <c r="G30" s="9"/>
       <c r="H30" s="9"/>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:17">
       <c r="B32" s="1" t="s">
         <v>53</v>
       </c>
@@ -3788,7 +4862,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6">
       <c r="A33" s="1" t="s">
         <v>155</v>
       </c>
@@ -3803,7 +4877,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" ht="16">
       <c r="B34" s="29" t="s">
         <v>149</v>
       </c>
@@ -3815,7 +4889,7 @@
       </c>
       <c r="E34" s="30"/>
     </row>
-    <row r="35" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" ht="16">
       <c r="B35" s="18" t="s">
         <v>150</v>
       </c>
@@ -3827,7 +4901,7 @@
       </c>
       <c r="E35" s="30"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6">
       <c r="B36" s="18" t="s">
         <v>150</v>
       </c>
@@ -3839,7 +4913,7 @@
       </c>
       <c r="E36" s="30"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6">
       <c r="B41" s="5">
         <v>190160099</v>
       </c>
@@ -3890,7 +4964,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E531EC0F-8B5B-B945-81ED-74853B083270}">
   <dimension ref="A1:R41"/>
   <sheetViews>
@@ -3898,14 +4972,14 @@
       <selection activeCell="J27" sqref="A1:J27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="5" width="10.83203125" style="1"/>
     <col min="6" max="6" width="26.6640625" style="1" customWidth="1"/>
     <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18">
       <c r="I1" s="9"/>
       <c r="J1" s="7"/>
       <c r="K1" s="30"/>
@@ -3917,7 +4991,7 @@
       <c r="Q1" s="30"/>
       <c r="R1" s="30"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18">
       <c r="A2" s="1" t="s">
         <v>158</v>
       </c>
@@ -3932,7 +5006,7 @@
       <c r="Q2" s="30"/>
       <c r="R2" s="30"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18">
       <c r="A3" s="30" t="s">
         <v>0</v>
       </c>
@@ -3968,7 +5042,7 @@
       <c r="Q3" s="30"/>
       <c r="R3" s="30"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18">
       <c r="A4" s="44" t="s">
         <v>5</v>
       </c>
@@ -4002,7 +5076,7 @@
       <c r="Q4" s="30"/>
       <c r="R4" s="30"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18">
       <c r="A5" s="30" t="s">
         <v>97</v>
       </c>
@@ -4038,7 +5112,7 @@
       <c r="Q5" s="30"/>
       <c r="R5" s="30"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18">
       <c r="A6" s="30" t="s">
         <v>15</v>
       </c>
@@ -4072,7 +5146,7 @@
       <c r="Q6" s="30"/>
       <c r="R6" s="30"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18">
       <c r="A7" s="30" t="s">
         <v>21</v>
       </c>
@@ -4108,7 +5182,7 @@
       <c r="Q7" s="30"/>
       <c r="R7" s="30"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18">
       <c r="A8" s="30" t="s">
         <v>26</v>
       </c>
@@ -4144,7 +5218,7 @@
       <c r="Q8" s="30"/>
       <c r="R8" s="30"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18">
       <c r="A9" s="30" t="s">
         <v>96</v>
       </c>
@@ -4180,7 +5254,7 @@
       <c r="Q9" s="30"/>
       <c r="R9" s="30"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18">
       <c r="A10" s="30" t="s">
         <v>32</v>
       </c>
@@ -4214,7 +5288,7 @@
       <c r="Q10" s="30"/>
       <c r="R10" s="30"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18">
       <c r="A11" s="30" t="s">
         <v>95</v>
       </c>
@@ -4250,7 +5324,7 @@
       <c r="Q11" s="30"/>
       <c r="R11" s="30"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18">
       <c r="A12" s="30" t="s">
         <v>41</v>
       </c>
@@ -4286,7 +5360,7 @@
       <c r="Q12" s="30"/>
       <c r="R12" s="30"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18">
       <c r="A13" s="30" t="s">
         <v>100</v>
       </c>
@@ -4320,7 +5394,7 @@
       <c r="Q13" s="30"/>
       <c r="R13" s="30"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18">
       <c r="A14" s="30"/>
       <c r="B14" s="30" t="s">
         <v>46</v>
@@ -4354,7 +5428,7 @@
       <c r="Q14" s="30"/>
       <c r="R14" s="30"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18">
       <c r="A15" s="30" t="s">
         <v>102</v>
       </c>
@@ -4392,7 +5466,7 @@
       <c r="Q15" s="30"/>
       <c r="R15" s="30"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18">
       <c r="A16" s="30" t="s">
         <v>82</v>
       </c>
@@ -4430,7 +5504,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18">
       <c r="A17" s="40" t="s">
         <v>136</v>
       </c>
@@ -4470,7 +5544,7 @@
       </c>
       <c r="R17" s="30"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18">
       <c r="A18" s="38" t="s">
         <v>51</v>
       </c>
@@ -4508,7 +5582,7 @@
       </c>
       <c r="R18" s="30"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:18">
       <c r="A19" s="38" t="s">
         <v>113</v>
       </c>
@@ -4544,7 +5618,7 @@
       </c>
       <c r="R19" s="30"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:18">
       <c r="A20" s="38" t="s">
         <v>132</v>
       </c>
@@ -4578,7 +5652,7 @@
       <c r="Q20" s="30"/>
       <c r="R20" s="30"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:18">
       <c r="A21" s="30" t="s">
         <v>133</v>
       </c>
@@ -4612,7 +5686,7 @@
       <c r="Q21" s="30"/>
       <c r="R21" s="30"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:18">
       <c r="A22" s="30" t="s">
         <v>134</v>
       </c>
@@ -4646,7 +5720,7 @@
       <c r="Q22" s="30"/>
       <c r="R22" s="30"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:18">
       <c r="A23" s="44" t="s">
         <v>67</v>
       </c>
@@ -4680,7 +5754,7 @@
       <c r="Q23" s="30"/>
       <c r="R23" s="30"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:18">
       <c r="I24" s="9"/>
       <c r="J24" s="9"/>
       <c r="K24" s="30"/>
@@ -4692,7 +5766,7 @@
       <c r="Q24" s="30"/>
       <c r="R24" s="30"/>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:18">
       <c r="A25" s="30" t="s">
         <v>159</v>
       </c>
@@ -4714,7 +5788,7 @@
       <c r="Q25" s="30"/>
       <c r="R25" s="30"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:18">
       <c r="A26" s="48" t="s">
         <v>138</v>
       </c>
@@ -4744,7 +5818,7 @@
       <c r="Q26" s="30"/>
       <c r="R26" s="30"/>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:18">
       <c r="I27" s="9"/>
       <c r="J27" s="7"/>
       <c r="K27" s="30"/>
@@ -4756,7 +5830,7 @@
       <c r="Q27" s="30"/>
       <c r="R27" s="30"/>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:18">
       <c r="I28" s="9"/>
       <c r="J28" s="9"/>
       <c r="L28" s="30"/>
@@ -4767,7 +5841,7 @@
       <c r="Q28" s="30"/>
       <c r="R28" s="30"/>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:18">
       <c r="A29" s="30"/>
       <c r="B29" s="30"/>
       <c r="C29" s="30"/>
@@ -4787,7 +5861,7 @@
       <c r="Q29" s="30"/>
       <c r="R29" s="30"/>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:18">
       <c r="A30" s="30"/>
       <c r="B30" s="30"/>
       <c r="C30" s="30"/>
@@ -4807,7 +5881,7 @@
       <c r="Q30" s="30"/>
       <c r="R30" s="30"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:18">
       <c r="A31" s="30"/>
       <c r="B31" s="30"/>
       <c r="C31" s="30"/>
@@ -4827,7 +5901,7 @@
       <c r="Q31" s="30"/>
       <c r="R31" s="30"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:18">
       <c r="A32" s="30"/>
       <c r="B32" s="30"/>
       <c r="C32" s="30"/>
@@ -4847,7 +5921,7 @@
       <c r="Q32" s="30"/>
       <c r="R32" s="30"/>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:18">
       <c r="A33" s="30"/>
       <c r="B33" s="18"/>
       <c r="C33" s="30"/>
@@ -4867,7 +5941,7 @@
       <c r="Q33" s="30"/>
       <c r="R33" s="30"/>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:18">
       <c r="A34" s="30"/>
       <c r="B34" s="29"/>
       <c r="C34" s="30"/>
@@ -4887,7 +5961,7 @@
       <c r="Q34" s="30"/>
       <c r="R34" s="30"/>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:18">
       <c r="A35" s="30"/>
       <c r="B35" s="18"/>
       <c r="C35" s="30"/>
@@ -4907,7 +5981,7 @@
       <c r="Q35" s="30"/>
       <c r="R35" s="30"/>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:18">
       <c r="A36" s="30"/>
       <c r="B36" s="18"/>
       <c r="C36" s="30"/>
@@ -4927,7 +6001,7 @@
       <c r="Q36" s="30"/>
       <c r="R36" s="30"/>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:18">
       <c r="A37" s="30"/>
       <c r="B37" s="30"/>
       <c r="C37" s="30"/>
@@ -4947,7 +6021,7 @@
       <c r="Q37" s="30"/>
       <c r="R37" s="30"/>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:18">
       <c r="A38" s="30"/>
       <c r="B38" s="30"/>
       <c r="C38" s="30"/>
@@ -4967,7 +6041,7 @@
       <c r="Q38" s="30"/>
       <c r="R38" s="30"/>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:18">
       <c r="A39" s="30"/>
       <c r="B39" s="30"/>
       <c r="C39" s="30"/>
@@ -4987,7 +6061,7 @@
       <c r="Q39" s="30"/>
       <c r="R39" s="30"/>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:18">
       <c r="A40" s="30"/>
       <c r="B40" s="30"/>
       <c r="C40" s="30"/>
@@ -5007,7 +6081,7 @@
       <c r="Q40" s="30"/>
       <c r="R40" s="30"/>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:18">
       <c r="A41" s="30"/>
       <c r="B41" s="37"/>
       <c r="C41" s="30"/>

</xml_diff>

<commit_message>
updated schematic, pre-new board layout
barrel shifter driving changes (MOSFETs)
</commit_message>
<xml_diff>
--- a/designs/Pufferfish-Interface-2/reference/Interface Bill of Materials v2-1.xlsx
+++ b/designs/Pufferfish-Interface-2/reference/Interface Bill of Materials v2-1.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurenadachi/Documents/GitHub/pufferfish-electronics/designs/Pufferfish-Interface-2/reference/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F24E66C-55C0-8E4E-A585-A2734672D1F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68B775DF-AE55-8148-AD03-8B3CE50E5D2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="25040" windowHeight="14040" xr2:uid="{AB4FADCF-5D3E-0F4F-A6DE-656B770204FC}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM Interface 2-3" sheetId="6" r:id="rId1"/>
-    <sheet name="BOM Interface" sheetId="3" r:id="rId2"/>
+    <sheet name="Microphone" sheetId="5" r:id="rId2"/>
     <sheet name="BOM Pi" sheetId="4" r:id="rId3"/>
-    <sheet name="BOM Interface 2-2" sheetId="5" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId5"/>
-    <sheet name="Digikey order" sheetId="2" r:id="rId6"/>
+    <sheet name="Digikey order" sheetId="2" r:id="rId4"/>
+    <sheet name="BOM Interface 2" sheetId="3" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="332">
   <si>
     <t>ID</t>
   </si>
@@ -752,9 +752,6 @@
   </si>
   <si>
     <t>https://www.digikey.com/product-detail/en/molex/0022272091/WM4118-ND/1130584</t>
-  </si>
-  <si>
-    <t>Contol board to Pi</t>
   </si>
   <si>
     <t>https://www.mouser.com/ProductDetail/TE-Connectivity/1-1658527-3?qs=3csLVnQQLU2jT%252BbogjRSzQ%3D%3D</t>
@@ -1048,12 +1045,87 @@
   <si>
     <t>A33165-ND</t>
   </si>
+  <si>
+    <t>MIC1</t>
+  </si>
+  <si>
+    <t>EM-6022P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Microphone for sensing alarm functionality </t>
+  </si>
+  <si>
+    <t>433-1088-ND</t>
+  </si>
+  <si>
+    <t>6mm dia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.4 mm height </t>
+  </si>
+  <si>
+    <t xml:space="preserve">12mm dia </t>
+  </si>
+  <si>
+    <t>4.30mm height</t>
+  </si>
+  <si>
+    <t>102-1286-ND</t>
+  </si>
+  <si>
+    <t>Option w 6; https://www.digikey.com/product-detail/en/te-connectivity-amp-connectors/5103308-6/A33167-ND/1114905</t>
+  </si>
+  <si>
+    <t>For testing w Control board V1: https://www.digikey.com/product-detail/en/amphenol-icc-fci/67996-420HLF/609-3221-ND/1878553</t>
+  </si>
+  <si>
+    <t>Q12</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/fairchild-semiconductor/PN2222ABU/PN2222AFS-ND/6534</t>
+  </si>
+  <si>
+    <t>PN2222AFS-ND</t>
+  </si>
+  <si>
+    <t>PN2222ABU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BJT (Alarm 2) </t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/?qs=84A%2FDAdkstKRjqrk64ONjg%3D%3D</t>
+  </si>
+  <si>
+    <t>Pi to cable</t>
+  </si>
+  <si>
+    <t>Cable to Control board</t>
+  </si>
+  <si>
+    <t>571-5103308-8</t>
+  </si>
+  <si>
+    <t>5103308-8</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/on-semiconductor/FDN352AP/FDN352APCT-ND/1849911</t>
+  </si>
+  <si>
+    <t>FDN352AP</t>
+  </si>
+  <si>
+    <t>Datasheet </t>
+  </si>
+  <si>
+    <t>MOSFETs (Barrel shifter PMOS)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="53">
+  <fonts count="54">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1340,6 +1412,13 @@
       <family val="2"/>
     </font>
     <font>
+      <b/>
+      <sz val="24"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color theme="6"/>
       <name val="Calibri"/>
@@ -1468,7 +1547,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
@@ -1564,22 +1643,23 @@
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="38" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="38" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="41" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="41" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="43" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="42" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="42" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="44" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="29" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
@@ -1897,10 +1977,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85374FF2-138F-FD4F-BB74-E6C88CA0C0BE}">
-  <dimension ref="A1:P30"/>
+  <dimension ref="A1:P33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="114" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
@@ -1918,7 +1998,7 @@
     <col min="12" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:16">
       <c r="A1" s="1" t="s">
         <v>225</v>
       </c>
@@ -1956,7 +2036,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:16">
       <c r="A2" s="55" t="s">
         <v>212</v>
       </c>
@@ -1988,7 +2068,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:16">
       <c r="A3" s="55" t="s">
         <v>213</v>
       </c>
@@ -2017,37 +2097,43 @@
         <v>452000</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
-      <c r="A4" s="93" t="s">
+    <row r="4" spans="1:16">
+      <c r="A4" s="94" t="s">
         <v>214</v>
       </c>
       <c r="B4" s="48" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="48" t="s">
-        <v>305</v>
-      </c>
-      <c r="D4" s="94">
+        <v>304</v>
+      </c>
+      <c r="D4" s="95">
         <v>1</v>
       </c>
       <c r="E4" s="48" t="s">
         <v>23</v>
       </c>
       <c r="F4" s="48" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="G4" s="49" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H4" s="48"/>
+      <c r="I4" s="1" t="s">
+        <v>317</v>
+      </c>
       <c r="J4" s="16">
         <v>2500</v>
       </c>
       <c r="K4" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:13">
+      <c r="O4" s="1" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
       <c r="A5" s="55" t="s">
         <v>215</v>
       </c>
@@ -2076,7 +2162,7 @@
         <v>49000</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:16">
       <c r="A6" s="55" t="s">
         <v>216</v>
       </c>
@@ -2114,7 +2200,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:16">
       <c r="A7" s="55" t="s">
         <v>217</v>
       </c>
@@ -2146,7 +2232,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:16">
       <c r="A8" s="55" t="s">
         <v>218</v>
       </c>
@@ -2172,7 +2258,7 @@
         <v>42000</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:16">
       <c r="A9" s="55" t="s">
         <v>219</v>
       </c>
@@ -2201,467 +2287,560 @@
         <v>75000</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
-      <c r="A10" s="55" t="s">
+    <row r="10" spans="1:16" ht="30">
+      <c r="A10" s="55"/>
+      <c r="C10" s="77" t="s">
+        <v>329</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="J10" s="16"/>
+    </row>
+    <row r="11" spans="1:16" ht="16">
+      <c r="A11" s="55" t="s">
         <v>220</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="22" t="s">
-        <v>177</v>
-      </c>
-      <c r="D10" s="2">
+      <c r="C11" s="53" t="s">
+        <v>330</v>
+      </c>
+      <c r="D11" s="2">
         <v>3</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F10" s="21" t="s">
+      <c r="F11" s="21" t="s">
         <v>176</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G11" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="J10" s="16"/>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="A11" s="55" t="s">
+      <c r="J11" s="16"/>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12" s="55"/>
+      <c r="B12" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>321</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="F12" s="21" t="s">
+        <v>320</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="J12" s="16"/>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13" s="55" t="s">
         <v>221</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B13" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C13" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D13" s="9">
         <f>4</f>
         <v>4</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E13" s="11">
         <v>82</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="F13" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G13" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="16">
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="16">
         <v>100000</v>
       </c>
     </row>
-    <row r="12" spans="1:13" s="9" customFormat="1">
-      <c r="A12" s="55" t="s">
+    <row r="14" spans="1:16">
+      <c r="A14" s="55" t="s">
         <v>222</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="B14" s="9"/>
+      <c r="C14" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D14" s="9">
         <f>10+6+8</f>
         <v>24</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E14" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="F14" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G14" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="H12" s="65"/>
-      <c r="I12" s="60"/>
-      <c r="J12" s="16"/>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="A13" s="55" t="s">
+      <c r="H14" s="65"/>
+      <c r="I14" s="60"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="9"/>
+    </row>
+    <row r="15" spans="1:16" s="9" customFormat="1">
+      <c r="A15" s="55" t="s">
         <v>223</v>
       </c>
-      <c r="B13" s="26" t="s">
+      <c r="B15" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="C13" s="72">
+      <c r="C15" s="72">
         <v>1718560009</v>
       </c>
-      <c r="D13" s="26">
-        <v>1</v>
-      </c>
-      <c r="E13" s="26" t="s">
+      <c r="D15" s="26">
+        <v>1</v>
+      </c>
+      <c r="E15" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="F13" s="21" t="s">
+      <c r="F15" s="21" t="s">
         <v>236</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="G15" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="H13" s="9" t="s">
+      <c r="H15" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="I13" s="9"/>
-      <c r="J13" s="16">
+      <c r="J15" s="16">
         <v>20390000</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" s="38" customFormat="1">
-      <c r="A14" s="55" t="s">
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="A16" s="55" t="s">
         <v>224</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C16" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="D14" s="9">
-        <v>1</v>
-      </c>
-      <c r="E14" s="9" t="s">
+      <c r="D16" s="9">
+        <v>1</v>
+      </c>
+      <c r="E16" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="F14" s="21" t="s">
+      <c r="F16" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="G16" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="H14" s="26" t="s">
+      <c r="H16" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="I14" s="26" t="s">
+      <c r="I16" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="J14" s="59">
+      <c r="J16" s="59">
         <v>4000</v>
       </c>
-      <c r="K14" s="38">
+      <c r="K16" s="38">
         <v>15</v>
       </c>
-      <c r="L14" s="38" t="s">
+      <c r="L16" s="38" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="15" spans="1:13">
-      <c r="B15" s="48" t="s">
+      <c r="M16" s="38"/>
+      <c r="N16" s="38"/>
+      <c r="O16" s="38"/>
+      <c r="P16" s="38"/>
+    </row>
+    <row r="17" spans="1:16" s="38" customFormat="1">
+      <c r="B17" s="48" t="s">
+        <v>302</v>
+      </c>
+      <c r="C17" s="41" t="s">
         <v>303</v>
       </c>
-      <c r="C15" s="41" t="s">
-        <v>304</v>
-      </c>
-      <c r="D15" s="48">
-        <v>1</v>
-      </c>
-      <c r="E15" s="44"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="49" t="s">
-        <v>302</v>
-      </c>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="16">
+      <c r="D17" s="48">
+        <v>1</v>
+      </c>
+      <c r="E17" s="44"/>
+      <c r="F17" s="21" t="s">
+        <v>315</v>
+      </c>
+      <c r="G17" s="49" t="s">
+        <v>301</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>313</v>
+      </c>
+      <c r="I17" s="21" t="s">
+        <v>314</v>
+      </c>
+      <c r="J17" s="16">
         <v>4500</v>
       </c>
-      <c r="K15" s="1">
+      <c r="K17" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="17" spans="1:16">
-      <c r="P17" s="29"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
     </row>
     <row r="18" spans="1:16">
-      <c r="A18" s="55" t="s">
-        <v>226</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="C18" s="22" t="s">
-        <v>150</v>
-      </c>
-      <c r="D18" s="2">
-        <v>1</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F18" s="25" t="s">
-        <v>130</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="I18" s="20" t="s">
-        <v>157</v>
-      </c>
-      <c r="J18" s="30" t="s">
-        <v>152</v>
-      </c>
-      <c r="P18" s="18"/>
-    </row>
-    <row r="19" spans="1:16">
-      <c r="A19" s="55" t="s">
-        <v>227</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C19" s="22" t="s">
-        <v>167</v>
-      </c>
-      <c r="D19" s="1">
-        <v>4</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="F19" s="21" t="s">
-        <v>168</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="L19" s="1" t="s">
-        <v>121</v>
+      <c r="B18" s="48" t="s">
+        <v>307</v>
+      </c>
+      <c r="C18" s="41" t="s">
+        <v>308</v>
+      </c>
+      <c r="D18" s="48">
+        <v>1</v>
+      </c>
+      <c r="E18" s="48" t="s">
+        <v>309</v>
+      </c>
+      <c r="F18" s="47" t="s">
+        <v>310</v>
+      </c>
+      <c r="G18" s="49" t="s">
+        <v>300</v>
+      </c>
+      <c r="H18" s="48" t="s">
+        <v>311</v>
+      </c>
+      <c r="I18" s="48" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="20" spans="1:16">
-      <c r="A20" s="55" t="s">
-        <v>228</v>
-      </c>
-      <c r="B20" s="26" t="s">
-        <v>133</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D20" s="1">
-        <v>1</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="H20" s="3"/>
-      <c r="J20" s="16">
-        <v>35000</v>
-      </c>
-      <c r="K20" s="1">
-        <v>15</v>
-      </c>
+      <c r="P20" s="29"/>
     </row>
     <row r="21" spans="1:16">
       <c r="A21" s="55" t="s">
-        <v>229</v>
-      </c>
-      <c r="B21" s="26" t="s">
-        <v>51</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>125</v>
+        <v>226</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C21" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="D21" s="2">
+        <v>1</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="F21" s="25" t="s">
         <v>130</v>
       </c>
-      <c r="G21" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="I21" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="J21" s="16"/>
+      <c r="G21" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="I21" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="J21" s="30" t="s">
+        <v>152</v>
+      </c>
       <c r="P21" s="18"/>
     </row>
     <row r="22" spans="1:16">
       <c r="A22" s="55" t="s">
-        <v>230</v>
-      </c>
-      <c r="B22" s="31" t="s">
-        <v>113</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="D22" s="32">
-        <v>1</v>
-      </c>
-      <c r="E22" s="32" t="s">
-        <v>62</v>
-      </c>
-      <c r="F22" s="32" t="s">
-        <v>161</v>
-      </c>
-      <c r="G22" s="58" t="s">
-        <v>76</v>
-      </c>
-      <c r="H22" s="32"/>
-      <c r="I22" s="34"/>
-      <c r="J22" s="17">
-        <v>60</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>137</v>
+        <v>227</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C22" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="D22" s="1">
+        <v>4</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F22" s="21" t="s">
+        <v>168</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="23" spans="1:16">
       <c r="A23" s="55" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B23" s="26" t="s">
-        <v>114</v>
-      </c>
-      <c r="C23" s="25" t="s">
-        <v>129</v>
-      </c>
-      <c r="F23" s="25" t="s">
-        <v>130</v>
+        <v>133</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" s="1">
+        <v>1</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="H23" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="J23" s="17">
-        <v>0</v>
+        <v>58</v>
+      </c>
+      <c r="H23" s="3"/>
+      <c r="J23" s="16">
+        <v>35000</v>
       </c>
       <c r="K23" s="1">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:16">
       <c r="A24" s="55" t="s">
-        <v>232</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="C24" s="22" t="s">
-        <v>171</v>
-      </c>
-      <c r="D24" s="1">
-        <v>3</v>
+        <v>229</v>
+      </c>
+      <c r="B24" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>125</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="F24" s="21" t="s">
-        <v>172</v>
-      </c>
-      <c r="G24" s="6" t="s">
-        <v>170</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="F24" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="I24" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="J24" s="16"/>
+      <c r="P24" s="18"/>
     </row>
     <row r="25" spans="1:16">
       <c r="A25" s="55" t="s">
-        <v>233</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D25" s="1">
-        <v>1</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="G25" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="J25" s="16">
-        <v>7500</v>
+        <v>230</v>
+      </c>
+      <c r="B25" s="31" t="s">
+        <v>113</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D25" s="32">
+        <v>1</v>
+      </c>
+      <c r="E25" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="F25" s="32" t="s">
+        <v>161</v>
+      </c>
+      <c r="G25" s="58" t="s">
+        <v>76</v>
+      </c>
+      <c r="H25" s="32"/>
+      <c r="I25" s="34"/>
+      <c r="J25" s="17">
+        <v>60</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="26" spans="1:16">
-      <c r="B26" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="D26" s="9">
-        <v>1</v>
-      </c>
-      <c r="E26" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="F26" s="9"/>
-      <c r="G26" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="H26" s="8"/>
-    </row>
-    <row r="27" spans="1:16" ht="13" customHeight="1">
+      <c r="A26" s="55" t="s">
+        <v>231</v>
+      </c>
+      <c r="B26" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="C26" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="F26" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="J26" s="17">
+        <v>0</v>
+      </c>
+      <c r="K26" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16">
+      <c r="A27" s="55" t="s">
+        <v>232</v>
+      </c>
       <c r="B27" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="C27" s="15" t="s">
+      <c r="C27" s="22" t="s">
+        <v>171</v>
+      </c>
+      <c r="D27" s="1">
+        <v>3</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="F27" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
+      <c r="A28" s="55" t="s">
+        <v>233</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D28" s="1">
+        <v>1</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="J28" s="16">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16">
+      <c r="B29" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D29" s="9">
+        <v>1</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="F29" s="9"/>
+      <c r="G29" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="H29" s="8"/>
+    </row>
+    <row r="30" spans="1:16" ht="13" customHeight="1">
+      <c r="B30" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C30" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="D27" s="1">
-        <v>1</v>
-      </c>
-      <c r="E27" s="1" t="s">
+      <c r="D30" s="1">
+        <v>1</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="F27" s="15"/>
-      <c r="G27" s="6"/>
-      <c r="J27" s="19">
+      <c r="F30" s="15"/>
+      <c r="G30" s="6"/>
+      <c r="J30" s="19">
         <v>758</v>
       </c>
-      <c r="K27" s="25" t="s">
+      <c r="K30" s="25" t="s">
         <v>128</v>
       </c>
-      <c r="L27" s="18" t="s">
+      <c r="L30" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="M27" s="1" t="s">
+      <c r="M30" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="30" spans="1:16">
-      <c r="K30" s="1">
+    <row r="33" spans="11:11">
+      <c r="K33" s="1">
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G9" r:id="rId1" display="https://www.digikey.com/product-detail/en/vishay-siliconix/2N7002E-T1-E3/2N7002E-T1-E3CT-ND/3946142?utm_adgroup=Semiconductor%20Modules&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Dynamic%20Search_RLSA_Buyers&amp;utm_term=&amp;utm_content=Semiconductor%20Modules&amp;gclid=Cj0KCQjwrIf3BRD1ARIsAMuugNtAYg0B4uzN6uG3FDVYlywiEKFAGbXRLO8hnfXG_d9twvCOg1_5j4waAs4CEALw_wcB" xr:uid="{78A24A15-31CF-9F47-A91F-FA441EF9C614}"/>
-    <hyperlink ref="G12" r:id="rId2" xr:uid="{73D98201-D87A-4B4B-A02A-29A5FAECD42E}"/>
-    <hyperlink ref="G20" r:id="rId3" xr:uid="{8CA4D74E-E935-2F42-93CC-3425476EDB88}"/>
+    <hyperlink ref="G14" r:id="rId2" xr:uid="{73D98201-D87A-4B4B-A02A-29A5FAECD42E}"/>
+    <hyperlink ref="G23" r:id="rId3" xr:uid="{8CA4D74E-E935-2F42-93CC-3425476EDB88}"/>
     <hyperlink ref="G3" r:id="rId4" xr:uid="{8791FA06-E3A4-1943-BFDF-87D3983EC694}"/>
     <hyperlink ref="G5" r:id="rId5" xr:uid="{03BF4570-C52E-B244-9F90-52764ADFD1C5}"/>
     <hyperlink ref="G8" r:id="rId6" xr:uid="{F9C832B3-42F8-D744-BBC6-D42227150E36}"/>
-    <hyperlink ref="G21" r:id="rId7" xr:uid="{F139212D-3876-314E-B9A8-32A838323003}"/>
+    <hyperlink ref="G24" r:id="rId7" xr:uid="{F139212D-3876-314E-B9A8-32A838323003}"/>
     <hyperlink ref="G6" r:id="rId8" xr:uid="{65E48627-1237-5243-A5A5-4DF4CF98D5E0}"/>
-    <hyperlink ref="G11" r:id="rId9" xr:uid="{51797C28-FED1-D443-9104-7306ACDF3AA3}"/>
-    <hyperlink ref="G14" r:id="rId10" xr:uid="{6AB19274-16AE-1F47-AA50-8E6B56033E01}"/>
-    <hyperlink ref="G25" r:id="rId11" xr:uid="{D37BCA5F-7D02-BC43-A9AF-97299644271B}"/>
-    <hyperlink ref="H23" r:id="rId12" xr:uid="{643D5EB8-96B1-8349-86E7-1106B7EEF44C}"/>
-    <hyperlink ref="G22" r:id="rId13" xr:uid="{3A799947-BEBC-EC4A-A0FF-D641DB274EDC}"/>
-    <hyperlink ref="G18" r:id="rId14" xr:uid="{D165C778-190D-4F4B-B93F-7CC39E60CF2D}"/>
+    <hyperlink ref="G13" r:id="rId9" xr:uid="{51797C28-FED1-D443-9104-7306ACDF3AA3}"/>
+    <hyperlink ref="G16" r:id="rId10" xr:uid="{6AB19274-16AE-1F47-AA50-8E6B56033E01}"/>
+    <hyperlink ref="G28" r:id="rId11" xr:uid="{D37BCA5F-7D02-BC43-A9AF-97299644271B}"/>
+    <hyperlink ref="H26" r:id="rId12" xr:uid="{643D5EB8-96B1-8349-86E7-1106B7EEF44C}"/>
+    <hyperlink ref="G25" r:id="rId13" xr:uid="{3A799947-BEBC-EC4A-A0FF-D641DB274EDC}"/>
+    <hyperlink ref="G21" r:id="rId14" xr:uid="{D165C778-190D-4F4B-B93F-7CC39E60CF2D}"/>
     <hyperlink ref="G7" r:id="rId15" xr:uid="{51412221-95CC-D040-BC45-2DF7E8EE65D6}"/>
-    <hyperlink ref="G10" r:id="rId16" display="https://www.digikey.com/product-detail/en/on-semiconductor/FDN337N/FDN337NCT-ND/458950?utm_adgroup=Semiconductor%20Modules&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Dynamic%20Search&amp;utm_term=&amp;utm_content=Semiconductor%20Modules&amp;gclid=EAIaIQobChMIi9eQ5_aJ6wIViZWzCh0mJgM4EAAYAyAAEgLjm_D_BwE" xr:uid="{4E70B157-27AD-0C43-B73B-B0A96F65C0B1}"/>
-    <hyperlink ref="G19" r:id="rId17" xr:uid="{CEF247F0-AC52-E148-9F68-14BD6BB6B45E}"/>
-    <hyperlink ref="G24" r:id="rId18" xr:uid="{01250BBC-38BA-5A4D-B165-4926E5F33703}"/>
+    <hyperlink ref="G11" r:id="rId16" display="https://www.digikey.com/product-detail/en/on-semiconductor/FDN337N/FDN337NCT-ND/458950?utm_adgroup=Semiconductor%20Modules&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Dynamic%20Search&amp;utm_term=&amp;utm_content=Semiconductor%20Modules&amp;gclid=EAIaIQobChMIi9eQ5_aJ6wIViZWzCh0mJgM4EAAYAyAAEgLjm_D_BwE" xr:uid="{4E70B157-27AD-0C43-B73B-B0A96F65C0B1}"/>
+    <hyperlink ref="G22" r:id="rId17" xr:uid="{CEF247F0-AC52-E148-9F68-14BD6BB6B45E}"/>
+    <hyperlink ref="G27" r:id="rId18" xr:uid="{01250BBC-38BA-5A4D-B165-4926E5F33703}"/>
+    <hyperlink ref="G18" r:id="rId19" xr:uid="{24693A1E-9A47-6144-87C0-3B9F1CA09FFF}"/>
+    <hyperlink ref="G17" r:id="rId20" xr:uid="{97A023A6-5A2C-B540-A54A-661583DFC3AB}"/>
+    <hyperlink ref="G12" r:id="rId21" xr:uid="{293D8BE5-40F8-464B-BD63-22CAE9653F27}"/>
+    <hyperlink ref="C11" r:id="rId22" display="https://www.onsemi.com/pub/Collateral/FDN352AP-D.pdf" xr:uid="{ABBE7E0D-6B11-8445-996D-3A0401273CEE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -2669,6 +2848,1831 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAC86840-D8AD-F542-98B2-FC57B25AE1B6}">
+  <dimension ref="A1:L21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="16384" width="10.83203125" style="74"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" s="74" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="74" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="74" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="74" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="74" t="s">
+        <v>78</v>
+      </c>
+      <c r="F1" s="74" t="s">
+        <v>119</v>
+      </c>
+      <c r="G1" s="74" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="74" t="s">
+        <v>266</v>
+      </c>
+      <c r="J1" s="74" t="s">
+        <v>270</v>
+      </c>
+      <c r="K1" s="74" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="84" t="s">
+        <v>242</v>
+      </c>
+      <c r="B2" s="84" t="s">
+        <v>268</v>
+      </c>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84" t="s">
+        <v>267</v>
+      </c>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84" t="s">
+        <v>275</v>
+      </c>
+      <c r="I2" s="84" t="s">
+        <v>269</v>
+      </c>
+      <c r="J2" s="84" t="s">
+        <v>276</v>
+      </c>
+      <c r="K2" s="85"/>
+      <c r="L2" s="81"/>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="81" t="s">
+        <v>243</v>
+      </c>
+      <c r="B3" s="82" t="s">
+        <v>272</v>
+      </c>
+      <c r="C3" s="81"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="81"/>
+      <c r="F3" s="81" t="s">
+        <v>271</v>
+      </c>
+      <c r="G3" s="83" t="s">
+        <v>273</v>
+      </c>
+      <c r="H3" s="81" t="s">
+        <v>251</v>
+      </c>
+      <c r="I3" s="81"/>
+      <c r="J3" s="81"/>
+      <c r="K3" s="81"/>
+      <c r="L3" s="81"/>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="84" t="s">
+        <v>136</v>
+      </c>
+      <c r="B4" s="84" t="s">
+        <v>244</v>
+      </c>
+      <c r="C4" s="84">
+        <v>1</v>
+      </c>
+      <c r="D4" s="84"/>
+      <c r="E4" s="84"/>
+      <c r="F4" s="84" t="s">
+        <v>257</v>
+      </c>
+      <c r="G4" s="87" t="s">
+        <v>274</v>
+      </c>
+      <c r="H4" s="84" t="s">
+        <v>254</v>
+      </c>
+      <c r="I4" s="81" t="s">
+        <v>258</v>
+      </c>
+      <c r="J4" s="81"/>
+      <c r="K4" s="86"/>
+      <c r="L4" s="81"/>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="78" t="s">
+        <v>245</v>
+      </c>
+      <c r="B5" s="78"/>
+      <c r="C5" s="78"/>
+      <c r="D5" s="78"/>
+      <c r="E5" s="78"/>
+      <c r="F5" s="78"/>
+      <c r="G5" s="78"/>
+      <c r="H5" s="78" t="s">
+        <v>256</v>
+      </c>
+      <c r="J5" s="74" t="s">
+        <v>280</v>
+      </c>
+      <c r="K5" s="80"/>
+      <c r="L5" s="74" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="74" t="s">
+        <v>250</v>
+      </c>
+      <c r="B6" s="75" t="s">
+        <v>246</v>
+      </c>
+      <c r="F6" s="74" t="s">
+        <v>259</v>
+      </c>
+      <c r="G6" s="74" t="s">
+        <v>260</v>
+      </c>
+      <c r="H6" s="74" t="s">
+        <v>252</v>
+      </c>
+      <c r="J6" s="74" t="s">
+        <v>262</v>
+      </c>
+      <c r="K6" s="79"/>
+      <c r="L6" s="88" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="74" t="s">
+        <v>247</v>
+      </c>
+      <c r="B7" s="74" t="s">
+        <v>248</v>
+      </c>
+      <c r="F7" s="74" t="s">
+        <v>261</v>
+      </c>
+      <c r="G7" s="76" t="s">
+        <v>265</v>
+      </c>
+      <c r="H7" s="74" t="s">
+        <v>255</v>
+      </c>
+      <c r="K7" s="79"/>
+      <c r="L7" s="88" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="B8" s="81" t="s">
+        <v>263</v>
+      </c>
+      <c r="C8" s="81"/>
+      <c r="D8" s="81" t="s">
+        <v>249</v>
+      </c>
+      <c r="E8" s="81"/>
+      <c r="F8" s="81" t="s">
+        <v>264</v>
+      </c>
+      <c r="G8" s="83" t="s">
+        <v>260</v>
+      </c>
+      <c r="H8" s="81" t="s">
+        <v>253</v>
+      </c>
+      <c r="I8" s="81"/>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="J11" s="74" t="s">
+        <v>283</v>
+      </c>
+      <c r="K11" s="89" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="19">
+      <c r="A12" s="74" t="s">
+        <v>195</v>
+      </c>
+      <c r="K12" s="90" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="19">
+      <c r="A13" s="74" t="s">
+        <v>196</v>
+      </c>
+      <c r="K13" s="91" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="J14" s="74" t="s">
+        <v>285</v>
+      </c>
+      <c r="K14" s="92" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="J15" s="93" t="s">
+        <v>287</v>
+      </c>
+      <c r="K15" s="74" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="J16" s="74" t="s">
+        <v>289</v>
+      </c>
+      <c r="K16" s="93" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="17" spans="10:11">
+      <c r="J17" s="74" t="s">
+        <v>290</v>
+      </c>
+      <c r="K17" s="92" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="18" spans="10:11">
+      <c r="J18" s="74" t="s">
+        <v>292</v>
+      </c>
+      <c r="K18" s="92" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="19" spans="10:11">
+      <c r="J19" s="74" t="s">
+        <v>294</v>
+      </c>
+      <c r="K19" s="92" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="20" spans="10:11">
+      <c r="J20" s="74" t="s">
+        <v>298</v>
+      </c>
+      <c r="K20" s="74" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="21" spans="10:11">
+      <c r="K21" s="74" t="s">
+        <v>300</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B81DA78-FD1B-474D-AB22-5A2533BD4F55}">
+  <dimension ref="A1:O17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:15">
+      <c r="A1" s="66" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="B3" s="67" t="s">
+        <v>194</v>
+      </c>
+      <c r="C3" s="9">
+        <v>1</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" s="9"/>
+      <c r="F3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G3" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="H3" s="68" t="s">
+        <v>73</v>
+      </c>
+      <c r="I3" s="17">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="C4" s="9">
+        <v>1</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="E4" s="9"/>
+      <c r="F4" s="56" t="s">
+        <v>66</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="H4" s="9"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="B5" s="69" t="s">
+        <v>188</v>
+      </c>
+      <c r="C5" s="9">
+        <v>1</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="E5" s="7"/>
+      <c r="F5" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9">
+        <v>3</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" s="70" t="s">
+        <v>107</v>
+      </c>
+      <c r="C8" s="9">
+        <v>1</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>200</v>
+      </c>
+      <c r="E8" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="C9" s="2">
+        <v>2</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="E9" s="24" t="s">
+        <v>182</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="B10" s="70" t="s">
+        <v>185</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="E10" s="24" t="s">
+        <v>184</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="B11" s="9"/>
+      <c r="C11" s="7">
+        <v>2</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9">
+        <v>1</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9">
+        <v>1</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9">
+        <v>3</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:15" ht="23">
+      <c r="A15" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="B15" s="71" t="s">
+        <v>234</v>
+      </c>
+      <c r="C15" s="9">
+        <v>1</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="E15" s="9"/>
+      <c r="F15" s="56" t="s">
+        <v>206</v>
+      </c>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:15" ht="17">
+      <c r="A16" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="B16" s="73" t="s">
+        <v>239</v>
+      </c>
+      <c r="C16" s="9">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>324</v>
+      </c>
+      <c r="E16" s="73" t="s">
+        <v>240</v>
+      </c>
+      <c r="F16" t="s">
+        <v>238</v>
+      </c>
+      <c r="O16" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="23">
+      <c r="A17" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="B17" s="71" t="s">
+        <v>327</v>
+      </c>
+      <c r="C17" s="9">
+        <v>1</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>325</v>
+      </c>
+      <c r="E17" s="73" t="s">
+        <v>326</v>
+      </c>
+      <c r="F17" t="s">
+        <v>323</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F3" r:id="rId1" xr:uid="{74B93430-441E-8349-BC5E-F7F0E84239A0}"/>
+    <hyperlink ref="F8" r:id="rId2" xr:uid="{234397FD-824F-A940-ABD9-42FA04BDB109}"/>
+    <hyperlink ref="F10" r:id="rId3" xr:uid="{3BC20B03-E28F-284C-98C9-689F7D8F5BDC}"/>
+    <hyperlink ref="F9" r:id="rId4" xr:uid="{0B16819B-B6C5-B443-83E4-E64E7575DBC5}"/>
+    <hyperlink ref="G3" r:id="rId5" xr:uid="{9E64481A-21B7-FA40-B839-4527BAD6F368}"/>
+    <hyperlink ref="F11" r:id="rId6" xr:uid="{FBA39D92-E9B8-B947-807D-B92B1457E13D}"/>
+    <hyperlink ref="F15" r:id="rId7" xr:uid="{CDC9A383-0E44-8744-9D39-55354FD83AA5}"/>
+    <hyperlink ref="F4" r:id="rId8" xr:uid="{F9D7AFCB-4795-3647-9ED8-EB4EF101C7E7}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E531EC0F-8B5B-B945-81ED-74853B083270}">
+  <dimension ref="A1:R41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
+  <cols>
+    <col min="1" max="5" width="10.83203125" style="1"/>
+    <col min="6" max="6" width="26.6640625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18">
+      <c r="I1" s="9"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="30"/>
+      <c r="Q1" s="30"/>
+      <c r="R1" s="30"/>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="I2" s="9"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="30"/>
+      <c r="R2" s="30"/>
+    </row>
+    <row r="3" spans="1:18">
+      <c r="A3" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="F3" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="G3" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="30"/>
+      <c r="I3" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="J3" s="7"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="30"/>
+      <c r="M3" s="30"/>
+      <c r="N3" s="30"/>
+      <c r="O3" s="30"/>
+      <c r="P3" s="30"/>
+      <c r="Q3" s="30"/>
+      <c r="R3" s="30"/>
+    </row>
+    <row r="4" spans="1:18">
+      <c r="A4" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="44">
+        <v>1</v>
+      </c>
+      <c r="D4" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="49" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="7">
+        <v>560</v>
+      </c>
+      <c r="J4" s="7"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
+      <c r="M4" s="30"/>
+      <c r="N4" s="30"/>
+      <c r="O4" s="30"/>
+      <c r="P4" s="30"/>
+      <c r="Q4" s="30"/>
+      <c r="R4" s="30"/>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="A5" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="B5" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="30">
+        <v>5</v>
+      </c>
+      <c r="D5" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="30"/>
+      <c r="I5" s="7">
+        <v>452000</v>
+      </c>
+      <c r="J5" s="7"/>
+      <c r="K5" s="30"/>
+      <c r="L5" s="30"/>
+      <c r="M5" s="30"/>
+      <c r="N5" s="30"/>
+      <c r="O5" s="30"/>
+      <c r="P5" s="30"/>
+      <c r="Q5" s="30"/>
+      <c r="R5" s="30"/>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="A6" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="30">
+        <v>1</v>
+      </c>
+      <c r="D6" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="36"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="7">
+        <v>2500</v>
+      </c>
+      <c r="J6" s="7"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="30"/>
+      <c r="M6" s="30"/>
+      <c r="N6" s="30"/>
+      <c r="O6" s="30"/>
+      <c r="P6" s="30"/>
+      <c r="Q6" s="30"/>
+      <c r="R6" s="30"/>
+    </row>
+    <row r="7" spans="1:18">
+      <c r="A7" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="30">
+        <v>1</v>
+      </c>
+      <c r="D7" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="30"/>
+      <c r="I7" s="7">
+        <v>49000</v>
+      </c>
+      <c r="J7" s="7"/>
+      <c r="K7" s="30"/>
+      <c r="L7" s="30"/>
+      <c r="M7" s="30"/>
+      <c r="N7" s="30"/>
+      <c r="O7" s="30"/>
+      <c r="P7" s="30"/>
+      <c r="Q7" s="30"/>
+      <c r="R7" s="30"/>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="A8" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" s="30">
+        <v>1</v>
+      </c>
+      <c r="D8" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="G8" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="30"/>
+      <c r="I8" s="7">
+        <v>684</v>
+      </c>
+      <c r="J8" s="7"/>
+      <c r="K8" s="30"/>
+      <c r="L8" s="30"/>
+      <c r="M8" s="30"/>
+      <c r="N8" s="30"/>
+      <c r="O8" s="30"/>
+      <c r="P8" s="30"/>
+      <c r="Q8" s="30"/>
+      <c r="R8" s="30"/>
+    </row>
+    <row r="9" spans="1:18">
+      <c r="A9" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="B9" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="30">
+        <v>2</v>
+      </c>
+      <c r="D9" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="36" t="s">
+        <v>112</v>
+      </c>
+      <c r="G9" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9" s="30"/>
+      <c r="I9" s="7">
+        <v>17500</v>
+      </c>
+      <c r="J9" s="7"/>
+      <c r="K9" s="30"/>
+      <c r="L9" s="30"/>
+      <c r="M9" s="30"/>
+      <c r="N9" s="30"/>
+      <c r="O9" s="30"/>
+      <c r="P9" s="30"/>
+      <c r="Q9" s="30"/>
+      <c r="R9" s="30"/>
+    </row>
+    <row r="10" spans="1:18">
+      <c r="A10" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="30">
+        <v>5</v>
+      </c>
+      <c r="D10" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="36"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="7">
+        <v>42000</v>
+      </c>
+      <c r="J10" s="7"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="30"/>
+      <c r="N10" s="30"/>
+      <c r="O10" s="30"/>
+      <c r="P10" s="30"/>
+      <c r="Q10" s="30"/>
+      <c r="R10" s="30"/>
+    </row>
+    <row r="11" spans="1:18">
+      <c r="A11" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="B11" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="30">
+        <v>7</v>
+      </c>
+      <c r="D11" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G11" s="36"/>
+      <c r="H11" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="I11" s="7">
+        <v>75000</v>
+      </c>
+      <c r="J11" s="7"/>
+      <c r="K11" s="30"/>
+      <c r="L11" s="30"/>
+      <c r="M11" s="30"/>
+      <c r="N11" s="30"/>
+      <c r="O11" s="30"/>
+      <c r="P11" s="30"/>
+      <c r="Q11" s="30"/>
+      <c r="R11" s="30"/>
+    </row>
+    <row r="12" spans="1:18">
+      <c r="A12" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="30">
+        <v>3</v>
+      </c>
+      <c r="D12" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" s="36"/>
+      <c r="H12" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="I12" s="7">
+        <v>283000</v>
+      </c>
+      <c r="J12" s="7"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="30"/>
+      <c r="M12" s="30"/>
+      <c r="N12" s="30"/>
+      <c r="O12" s="30"/>
+      <c r="P12" s="30"/>
+      <c r="Q12" s="30"/>
+      <c r="R12" s="30"/>
+    </row>
+    <row r="13" spans="1:18">
+      <c r="A13" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="B13" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="C13" s="30">
+        <v>4</v>
+      </c>
+      <c r="D13" s="37">
+        <v>82</v>
+      </c>
+      <c r="E13" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="G13" s="36"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="7">
+        <v>100000</v>
+      </c>
+      <c r="J13" s="7"/>
+      <c r="K13" s="30"/>
+      <c r="L13" s="30"/>
+      <c r="M13" s="30"/>
+      <c r="N13" s="30"/>
+      <c r="O13" s="30"/>
+      <c r="P13" s="30"/>
+      <c r="Q13" s="30"/>
+      <c r="R13" s="30"/>
+    </row>
+    <row r="14" spans="1:18">
+      <c r="A14" s="30"/>
+      <c r="B14" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="30">
+        <v>24</v>
+      </c>
+      <c r="D14" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="G14" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="H14" s="30"/>
+      <c r="I14" s="7">
+        <v>20390000</v>
+      </c>
+      <c r="J14" s="7"/>
+      <c r="K14" s="30"/>
+      <c r="L14" s="30"/>
+      <c r="M14" s="30"/>
+      <c r="N14" s="30"/>
+      <c r="O14" s="30"/>
+      <c r="P14" s="30"/>
+      <c r="Q14" s="30"/>
+      <c r="R14" s="30"/>
+    </row>
+    <row r="15" spans="1:18">
+      <c r="A15" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="B15" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="C15" s="30">
+        <v>1</v>
+      </c>
+      <c r="D15" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="E15" s="30" t="s">
+        <v>92</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="H15" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="I15" s="7">
+        <v>4000</v>
+      </c>
+      <c r="J15" s="7"/>
+      <c r="K15" s="30"/>
+      <c r="L15" s="30"/>
+      <c r="M15" s="30"/>
+      <c r="N15" s="30"/>
+      <c r="O15" s="30"/>
+      <c r="P15" s="30"/>
+      <c r="Q15" s="30"/>
+      <c r="R15" s="30"/>
+    </row>
+    <row r="16" spans="1:18">
+      <c r="A16" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="B16" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="C16" s="30">
+        <v>1</v>
+      </c>
+      <c r="D16" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="E16" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G16" s="36"/>
+      <c r="H16" s="36"/>
+      <c r="I16" s="7">
+        <v>4500</v>
+      </c>
+      <c r="J16" s="7"/>
+      <c r="K16" s="30"/>
+      <c r="L16" s="30"/>
+      <c r="M16" s="30"/>
+      <c r="N16" s="30"/>
+      <c r="O16" s="18"/>
+      <c r="P16" s="30" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q16" s="30"/>
+      <c r="R16" s="30" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18">
+      <c r="A17" s="40" t="s">
+        <v>136</v>
+      </c>
+      <c r="B17" s="41" t="s">
+        <v>150</v>
+      </c>
+      <c r="C17" s="40">
+        <v>1</v>
+      </c>
+      <c r="D17" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" s="42" t="s">
+        <v>130</v>
+      </c>
+      <c r="F17" s="50" t="s">
+        <v>156</v>
+      </c>
+      <c r="G17" s="51"/>
+      <c r="H17" s="43" t="s">
+        <v>157</v>
+      </c>
+      <c r="I17" s="52">
+        <v>2</v>
+      </c>
+      <c r="J17" s="7"/>
+      <c r="K17" s="30"/>
+      <c r="L17" s="30"/>
+      <c r="M17" s="30"/>
+      <c r="N17" s="30"/>
+      <c r="O17" s="29"/>
+      <c r="P17" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q17" s="30" t="s">
+        <v>147</v>
+      </c>
+      <c r="R17" s="30"/>
+    </row>
+    <row r="18" spans="1:18">
+      <c r="A18" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" s="39" t="s">
+        <v>125</v>
+      </c>
+      <c r="D18" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="E18" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="G18" s="36"/>
+      <c r="H18" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="30"/>
+      <c r="L18" s="30"/>
+      <c r="M18" s="30"/>
+      <c r="N18" s="30"/>
+      <c r="O18" s="18"/>
+      <c r="P18" s="30" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q18" s="30" t="s">
+        <v>152</v>
+      </c>
+      <c r="R18" s="30"/>
+    </row>
+    <row r="19" spans="1:18">
+      <c r="A19" s="38" t="s">
+        <v>113</v>
+      </c>
+      <c r="B19" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="E19" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="G19" s="36"/>
+      <c r="H19" s="36"/>
+      <c r="I19" s="7">
+        <v>60</v>
+      </c>
+      <c r="J19" s="7"/>
+      <c r="K19" s="30"/>
+      <c r="L19" s="30"/>
+      <c r="M19" s="30"/>
+      <c r="N19" s="30"/>
+      <c r="O19" s="18"/>
+      <c r="P19" s="30" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q19" s="30" t="s">
+        <v>153</v>
+      </c>
+      <c r="R19" s="30"/>
+    </row>
+    <row r="20" spans="1:18">
+      <c r="A20" s="38" t="s">
+        <v>132</v>
+      </c>
+      <c r="B20" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="C20" s="30">
+        <v>1</v>
+      </c>
+      <c r="D20" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="E20" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="G20" s="30"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="23">
+        <v>758</v>
+      </c>
+      <c r="J20" s="7"/>
+      <c r="K20" s="22"/>
+      <c r="L20" s="30"/>
+      <c r="M20" s="30"/>
+      <c r="N20" s="30"/>
+      <c r="O20" s="30"/>
+      <c r="P20" s="30"/>
+      <c r="Q20" s="30"/>
+      <c r="R20" s="30"/>
+    </row>
+    <row r="21" spans="1:18">
+      <c r="A21" s="30" t="s">
+        <v>133</v>
+      </c>
+      <c r="B21" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="30">
+        <v>1</v>
+      </c>
+      <c r="D21" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="E21" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="G21" s="36"/>
+      <c r="H21" s="36"/>
+      <c r="I21" s="7">
+        <v>35000</v>
+      </c>
+      <c r="J21" s="7"/>
+      <c r="K21" s="30"/>
+      <c r="L21" s="30"/>
+      <c r="M21" s="30"/>
+      <c r="N21" s="30"/>
+      <c r="O21" s="30"/>
+      <c r="P21" s="30"/>
+      <c r="Q21" s="30"/>
+      <c r="R21" s="30"/>
+    </row>
+    <row r="22" spans="1:18">
+      <c r="A22" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="B22" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="C22" s="30">
+        <v>1</v>
+      </c>
+      <c r="D22" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="E22" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="G22" s="36"/>
+      <c r="H22" s="36"/>
+      <c r="I22" s="7">
+        <v>7500</v>
+      </c>
+      <c r="J22" s="7"/>
+      <c r="K22" s="30"/>
+      <c r="L22" s="30"/>
+      <c r="M22" s="30"/>
+      <c r="N22" s="30"/>
+      <c r="O22" s="30"/>
+      <c r="P22" s="30"/>
+      <c r="Q22" s="30"/>
+      <c r="R22" s="30"/>
+    </row>
+    <row r="23" spans="1:18">
+      <c r="A23" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" s="41" t="s">
+        <v>107</v>
+      </c>
+      <c r="C23" s="44">
+        <v>1</v>
+      </c>
+      <c r="D23" s="46" t="s">
+        <v>108</v>
+      </c>
+      <c r="E23" s="47" t="s">
+        <v>109</v>
+      </c>
+      <c r="F23" s="49" t="s">
+        <v>122</v>
+      </c>
+      <c r="G23" s="45"/>
+      <c r="H23" s="44" t="s">
+        <v>139</v>
+      </c>
+      <c r="I23" s="7">
+        <v>15000</v>
+      </c>
+      <c r="J23" s="9"/>
+      <c r="M23" s="30"/>
+      <c r="N23" s="30"/>
+      <c r="O23" s="30"/>
+      <c r="P23" s="30"/>
+      <c r="Q23" s="30"/>
+      <c r="R23" s="30"/>
+    </row>
+    <row r="24" spans="1:18">
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="30"/>
+      <c r="L24" s="30"/>
+      <c r="M24" s="30"/>
+      <c r="N24" s="30"/>
+      <c r="O24" s="30"/>
+      <c r="P24" s="30"/>
+      <c r="Q24" s="30"/>
+      <c r="R24" s="30"/>
+    </row>
+    <row r="25" spans="1:18">
+      <c r="A25" s="30" t="s">
+        <v>159</v>
+      </c>
+      <c r="B25" s="20"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="30"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="30"/>
+      <c r="L25" s="30"/>
+      <c r="M25" s="30"/>
+      <c r="N25" s="30"/>
+      <c r="O25" s="30"/>
+      <c r="P25" s="30"/>
+      <c r="Q25" s="30"/>
+      <c r="R25" s="30"/>
+    </row>
+    <row r="26" spans="1:18">
+      <c r="A26" s="48" t="s">
+        <v>138</v>
+      </c>
+      <c r="B26" s="48" t="s">
+        <v>141</v>
+      </c>
+      <c r="C26" s="48">
+        <v>1</v>
+      </c>
+      <c r="D26" s="48" t="s">
+        <v>140</v>
+      </c>
+      <c r="E26" s="48"/>
+      <c r="F26" s="49" t="s">
+        <v>146</v>
+      </c>
+      <c r="G26" s="48"/>
+      <c r="H26" s="48"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="30"/>
+      <c r="L26" s="30"/>
+      <c r="M26" s="30"/>
+      <c r="N26" s="30"/>
+      <c r="O26" s="30"/>
+      <c r="P26" s="30"/>
+      <c r="Q26" s="30"/>
+      <c r="R26" s="30"/>
+    </row>
+    <row r="27" spans="1:18">
+      <c r="I27" s="9"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="30"/>
+      <c r="L27" s="30"/>
+      <c r="M27" s="30"/>
+      <c r="N27" s="30"/>
+      <c r="O27" s="30"/>
+      <c r="P27" s="30"/>
+      <c r="Q27" s="30"/>
+      <c r="R27" s="30"/>
+    </row>
+    <row r="28" spans="1:18">
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+      <c r="L28" s="30"/>
+      <c r="M28" s="30"/>
+      <c r="N28" s="30"/>
+      <c r="O28" s="30"/>
+      <c r="P28" s="30"/>
+      <c r="Q28" s="30"/>
+      <c r="R28" s="30"/>
+    </row>
+    <row r="29" spans="1:18">
+      <c r="A29" s="30"/>
+      <c r="B29" s="30"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="30"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="30"/>
+      <c r="J29" s="30"/>
+      <c r="K29" s="30"/>
+      <c r="L29" s="30"/>
+      <c r="M29" s="30"/>
+      <c r="N29" s="30"/>
+      <c r="O29" s="30"/>
+      <c r="P29" s="30"/>
+      <c r="Q29" s="30"/>
+      <c r="R29" s="30"/>
+    </row>
+    <row r="30" spans="1:18">
+      <c r="A30" s="30"/>
+      <c r="B30" s="30"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="30"/>
+      <c r="H30" s="30"/>
+      <c r="I30" s="30"/>
+      <c r="J30" s="30"/>
+      <c r="K30" s="30"/>
+      <c r="L30" s="30"/>
+      <c r="M30" s="30"/>
+      <c r="N30" s="30"/>
+      <c r="O30" s="30"/>
+      <c r="P30" s="30"/>
+      <c r="Q30" s="30"/>
+      <c r="R30" s="30"/>
+    </row>
+    <row r="31" spans="1:18">
+      <c r="A31" s="30"/>
+      <c r="B31" s="30"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="30"/>
+      <c r="F31" s="30"/>
+      <c r="G31" s="30"/>
+      <c r="H31" s="30"/>
+      <c r="I31" s="30"/>
+      <c r="J31" s="30"/>
+      <c r="K31" s="30"/>
+      <c r="L31" s="30"/>
+      <c r="M31" s="30"/>
+      <c r="N31" s="30"/>
+      <c r="O31" s="30"/>
+      <c r="P31" s="30"/>
+      <c r="Q31" s="30"/>
+      <c r="R31" s="30"/>
+    </row>
+    <row r="32" spans="1:18">
+      <c r="A32" s="30"/>
+      <c r="B32" s="30"/>
+      <c r="C32" s="30"/>
+      <c r="D32" s="30"/>
+      <c r="E32" s="30"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="36"/>
+      <c r="H32" s="36"/>
+      <c r="I32" s="28"/>
+      <c r="J32" s="30"/>
+      <c r="K32" s="30"/>
+      <c r="L32" s="30"/>
+      <c r="M32" s="30"/>
+      <c r="N32" s="30"/>
+      <c r="O32" s="30"/>
+      <c r="P32" s="30"/>
+      <c r="Q32" s="30"/>
+      <c r="R32" s="30"/>
+    </row>
+    <row r="33" spans="1:18">
+      <c r="A33" s="30"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="30"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="30"/>
+      <c r="F33" s="30"/>
+      <c r="G33" s="30"/>
+      <c r="H33" s="30"/>
+      <c r="I33" s="30"/>
+      <c r="J33" s="30"/>
+      <c r="K33" s="30"/>
+      <c r="L33" s="30"/>
+      <c r="M33" s="30"/>
+      <c r="N33" s="30"/>
+      <c r="O33" s="30"/>
+      <c r="P33" s="30"/>
+      <c r="Q33" s="30"/>
+      <c r="R33" s="30"/>
+    </row>
+    <row r="34" spans="1:18">
+      <c r="A34" s="30"/>
+      <c r="B34" s="29"/>
+      <c r="C34" s="30"/>
+      <c r="D34" s="30"/>
+      <c r="E34" s="30"/>
+      <c r="F34" s="30"/>
+      <c r="G34" s="30"/>
+      <c r="H34" s="30"/>
+      <c r="I34" s="30"/>
+      <c r="J34" s="30"/>
+      <c r="K34" s="30"/>
+      <c r="L34" s="30"/>
+      <c r="M34" s="30"/>
+      <c r="N34" s="30"/>
+      <c r="O34" s="30"/>
+      <c r="P34" s="30"/>
+      <c r="Q34" s="30"/>
+      <c r="R34" s="30"/>
+    </row>
+    <row r="35" spans="1:18">
+      <c r="A35" s="30"/>
+      <c r="B35" s="18"/>
+      <c r="C35" s="30"/>
+      <c r="D35" s="30"/>
+      <c r="E35" s="30"/>
+      <c r="F35" s="30"/>
+      <c r="G35" s="30"/>
+      <c r="H35" s="30"/>
+      <c r="I35" s="30"/>
+      <c r="J35" s="30"/>
+      <c r="K35" s="30"/>
+      <c r="L35" s="30"/>
+      <c r="M35" s="30"/>
+      <c r="N35" s="30"/>
+      <c r="O35" s="30"/>
+      <c r="P35" s="30"/>
+      <c r="Q35" s="30"/>
+      <c r="R35" s="30"/>
+    </row>
+    <row r="36" spans="1:18">
+      <c r="A36" s="30"/>
+      <c r="B36" s="18"/>
+      <c r="C36" s="30"/>
+      <c r="D36" s="30"/>
+      <c r="E36" s="30"/>
+      <c r="F36" s="30"/>
+      <c r="G36" s="30"/>
+      <c r="H36" s="30"/>
+      <c r="I36" s="30"/>
+      <c r="J36" s="30"/>
+      <c r="K36" s="30"/>
+      <c r="L36" s="30"/>
+      <c r="M36" s="30"/>
+      <c r="N36" s="30"/>
+      <c r="O36" s="30"/>
+      <c r="P36" s="30"/>
+      <c r="Q36" s="30"/>
+      <c r="R36" s="30"/>
+    </row>
+    <row r="37" spans="1:18">
+      <c r="A37" s="30"/>
+      <c r="B37" s="30"/>
+      <c r="C37" s="30"/>
+      <c r="D37" s="30"/>
+      <c r="E37" s="30"/>
+      <c r="F37" s="30"/>
+      <c r="G37" s="30"/>
+      <c r="H37" s="30"/>
+      <c r="I37" s="30"/>
+      <c r="J37" s="30"/>
+      <c r="K37" s="30"/>
+      <c r="L37" s="30"/>
+      <c r="M37" s="30"/>
+      <c r="N37" s="30"/>
+      <c r="O37" s="30"/>
+      <c r="P37" s="30"/>
+      <c r="Q37" s="30"/>
+      <c r="R37" s="30"/>
+    </row>
+    <row r="38" spans="1:18">
+      <c r="A38" s="30"/>
+      <c r="B38" s="30"/>
+      <c r="C38" s="30"/>
+      <c r="D38" s="30"/>
+      <c r="E38" s="30"/>
+      <c r="F38" s="30"/>
+      <c r="G38" s="30"/>
+      <c r="H38" s="30"/>
+      <c r="I38" s="30"/>
+      <c r="J38" s="30"/>
+      <c r="K38" s="30"/>
+      <c r="L38" s="30"/>
+      <c r="M38" s="30"/>
+      <c r="N38" s="30"/>
+      <c r="O38" s="30"/>
+      <c r="P38" s="30"/>
+      <c r="Q38" s="30"/>
+      <c r="R38" s="30"/>
+    </row>
+    <row r="39" spans="1:18">
+      <c r="A39" s="30"/>
+      <c r="B39" s="30"/>
+      <c r="C39" s="30"/>
+      <c r="D39" s="30"/>
+      <c r="E39" s="30"/>
+      <c r="F39" s="30"/>
+      <c r="G39" s="30"/>
+      <c r="H39" s="30"/>
+      <c r="I39" s="30"/>
+      <c r="J39" s="30"/>
+      <c r="K39" s="30"/>
+      <c r="L39" s="30"/>
+      <c r="M39" s="30"/>
+      <c r="N39" s="30"/>
+      <c r="O39" s="30"/>
+      <c r="P39" s="30"/>
+      <c r="Q39" s="30"/>
+      <c r="R39" s="30"/>
+    </row>
+    <row r="40" spans="1:18">
+      <c r="A40" s="30"/>
+      <c r="B40" s="30"/>
+      <c r="C40" s="30"/>
+      <c r="D40" s="30"/>
+      <c r="E40" s="30"/>
+      <c r="F40" s="30"/>
+      <c r="G40" s="30"/>
+      <c r="H40" s="30"/>
+      <c r="I40" s="30"/>
+      <c r="J40" s="30"/>
+      <c r="K40" s="30"/>
+      <c r="L40" s="30"/>
+      <c r="M40" s="30"/>
+      <c r="N40" s="30"/>
+      <c r="O40" s="30"/>
+      <c r="P40" s="30"/>
+      <c r="Q40" s="30"/>
+      <c r="R40" s="30"/>
+    </row>
+    <row r="41" spans="1:18">
+      <c r="A41" s="30"/>
+      <c r="B41" s="37"/>
+      <c r="C41" s="30"/>
+      <c r="D41" s="30"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="36"/>
+      <c r="H41" s="36"/>
+      <c r="I41" s="30"/>
+      <c r="J41" s="30"/>
+      <c r="K41" s="30"/>
+      <c r="L41" s="30"/>
+      <c r="M41" s="30"/>
+      <c r="N41" s="30"/>
+      <c r="O41" s="30"/>
+      <c r="P41" s="30"/>
+      <c r="Q41" s="30"/>
+      <c r="R41" s="30"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F4" r:id="rId1" xr:uid="{8D1A619E-9515-524F-B85A-A336184FAF79}"/>
+    <hyperlink ref="F5" r:id="rId2" xr:uid="{3AAC0776-E199-2D4D-A06E-B69343AE631B}"/>
+    <hyperlink ref="F6" r:id="rId3" xr:uid="{E461B325-C0F0-DA45-BDA8-84250934722A}"/>
+    <hyperlink ref="F7" r:id="rId4" xr:uid="{A60C7027-4B10-1E42-84BA-150AC300C862}"/>
+    <hyperlink ref="F8" r:id="rId5" xr:uid="{A1B92DA8-9C86-894C-993F-E8279B7DC277}"/>
+    <hyperlink ref="F10" r:id="rId6" xr:uid="{2515C9A8-0A71-A542-9DE7-C8FE503FC70A}"/>
+    <hyperlink ref="F11" r:id="rId7" display="https://www.digikey.com/product-detail/en/vishay-siliconix/2N7002E-T1-E3/2N7002E-T1-E3CT-ND/3946142?utm_adgroup=Semiconductor%20Modules&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Dynamic%20Search_RLSA_Buyers&amp;utm_term=&amp;utm_content=Semiconductor%20Modules&amp;gclid=Cj0KCQjwrIf3BRD1ARIsAMuugNtAYg0B4uzN6uG3FDVYlywiEKFAGbXRLO8hnfXG_d9twvCOg1_5j4waAs4CEALw_wcB" xr:uid="{E2ADDD7B-C275-A94E-8AEE-3CE4B10DEC4C}"/>
+    <hyperlink ref="F12" r:id="rId8" xr:uid="{27125482-B106-0147-B5B6-DE477125A0DC}"/>
+    <hyperlink ref="F13" r:id="rId9" xr:uid="{4CA4B337-CA91-E94E-B1F9-390ABAD5A837}"/>
+    <hyperlink ref="F14" r:id="rId10" xr:uid="{C48CA423-8ACC-8844-A5D3-14CB3B73FE20}"/>
+    <hyperlink ref="F15" r:id="rId11" xr:uid="{09C32FBB-C794-C744-A726-DDD0502B59F8}"/>
+    <hyperlink ref="F16" r:id="rId12" xr:uid="{C74B4AAC-4139-E74C-AA5B-14D06E76C48A}"/>
+    <hyperlink ref="F17" r:id="rId13" display="https://www.digikey.com/product-detail/en/inspired-led-llc/12V-SB-RGB-5M/1647-1069-2-ND/9091794" xr:uid="{BE2E3CAA-1537-B94B-BB1B-68FD97458555}"/>
+    <hyperlink ref="F18" r:id="rId14" xr:uid="{FD5CF46B-0193-D147-9826-48512F9DED48}"/>
+    <hyperlink ref="F19" r:id="rId15" xr:uid="{B100B64A-F971-F14A-ADEA-BBCFCD09A1AA}"/>
+    <hyperlink ref="F20" r:id="rId16" display="https://www.digikey.com/products/en?keywords=1658623-3" xr:uid="{1726C16B-1136-D04D-BE50-29799826E622}"/>
+    <hyperlink ref="F21" r:id="rId17" xr:uid="{646AFD14-92B1-D340-840C-800535B95EDE}"/>
+    <hyperlink ref="F22" r:id="rId18" xr:uid="{6AB34C14-18FE-564D-AEBF-20FEAB9DBCA9}"/>
+    <hyperlink ref="F23" r:id="rId19" display="https://www.digikey.com/product-detail/en/soberton-inc/SP-1504/433-1106-ND/3973690" xr:uid="{53C14038-FF08-BA49-8774-52E06C0F3358}"/>
+    <hyperlink ref="F26" r:id="rId20" xr:uid="{D34A9D3D-0E41-7C45-9FAE-64E42873741D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E9B5640-6FAA-8446-9BE8-A4CA60B8E992}">
   <dimension ref="A1:P30"/>
   <sheetViews>
@@ -3452,648 +5456,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B81DA78-FD1B-474D-AB22-5A2533BD4F55}">
-  <dimension ref="A1:O16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <sheetData>
-    <row r="1" spans="1:15">
-      <c r="A1" s="66" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:15">
-      <c r="A3" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="B3" s="67" t="s">
-        <v>194</v>
-      </c>
-      <c r="C3" s="9">
-        <v>1</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="E3" s="9"/>
-      <c r="F3" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="G3" s="56" t="s">
-        <v>65</v>
-      </c>
-      <c r="H3" s="68" t="s">
-        <v>73</v>
-      </c>
-      <c r="I3" s="17">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15">
-      <c r="A4" s="9" t="s">
-        <v>199</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>193</v>
-      </c>
-      <c r="C4" s="9">
-        <v>1</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>189</v>
-      </c>
-      <c r="E4" s="9"/>
-      <c r="F4" s="56" t="s">
-        <v>66</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>192</v>
-      </c>
-      <c r="H4" s="9"/>
-      <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:15">
-      <c r="A5" s="9" t="s">
-        <v>197</v>
-      </c>
-      <c r="B5" s="69" t="s">
-        <v>188</v>
-      </c>
-      <c r="C5" s="9">
-        <v>1</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>190</v>
-      </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="9" t="s">
-        <v>191</v>
-      </c>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:15">
-      <c r="A6" s="9" t="s">
-        <v>195</v>
-      </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9">
-        <v>3</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:15">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:15">
-      <c r="A8" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="B8" s="70" t="s">
-        <v>107</v>
-      </c>
-      <c r="C8" s="9">
-        <v>1</v>
-      </c>
-      <c r="D8" s="23" t="s">
-        <v>200</v>
-      </c>
-      <c r="E8" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="I8" s="1"/>
-    </row>
-    <row r="9" spans="1:15">
-      <c r="A9" s="9" t="s">
-        <v>197</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="C9" s="2">
-        <v>2</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>204</v>
-      </c>
-      <c r="E9" s="24" t="s">
-        <v>182</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="1"/>
-    </row>
-    <row r="10" spans="1:15">
-      <c r="A10" s="9" t="s">
-        <v>198</v>
-      </c>
-      <c r="B10" s="70" t="s">
-        <v>185</v>
-      </c>
-      <c r="C10" s="2">
-        <v>1</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="E10" s="24" t="s">
-        <v>184</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="1:15">
-      <c r="A11" s="9" t="s">
-        <v>195</v>
-      </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="7">
-        <v>2</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="1"/>
-    </row>
-    <row r="12" spans="1:15">
-      <c r="A12" s="9" t="s">
-        <v>195</v>
-      </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9">
-        <v>1</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="1"/>
-    </row>
-    <row r="13" spans="1:15">
-      <c r="A13" s="9" t="s">
-        <v>196</v>
-      </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9">
-        <v>1</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="1"/>
-    </row>
-    <row r="14" spans="1:15">
-      <c r="A14" s="9" t="s">
-        <v>196</v>
-      </c>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9">
-        <v>3</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="1"/>
-    </row>
-    <row r="15" spans="1:15" ht="23">
-      <c r="A15" s="9" t="s">
-        <v>197</v>
-      </c>
-      <c r="B15" s="71" t="s">
-        <v>234</v>
-      </c>
-      <c r="C15" s="9">
-        <v>1</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>205</v>
-      </c>
-      <c r="E15" s="9"/>
-      <c r="F15" s="56" t="s">
-        <v>206</v>
-      </c>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="1"/>
-    </row>
-    <row r="16" spans="1:15" ht="17">
-      <c r="A16" s="9" t="s">
-        <v>197</v>
-      </c>
-      <c r="B16" s="73" t="s">
-        <v>240</v>
-      </c>
-      <c r="C16" s="9">
-        <v>1</v>
-      </c>
-      <c r="D16" t="s">
-        <v>238</v>
-      </c>
-      <c r="E16" s="73" t="s">
-        <v>241</v>
-      </c>
-      <c r="F16" t="s">
-        <v>239</v>
-      </c>
-      <c r="O16" t="s">
-        <v>242</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1" xr:uid="{74B93430-441E-8349-BC5E-F7F0E84239A0}"/>
-    <hyperlink ref="F8" r:id="rId2" xr:uid="{234397FD-824F-A940-ABD9-42FA04BDB109}"/>
-    <hyperlink ref="F10" r:id="rId3" xr:uid="{3BC20B03-E28F-284C-98C9-689F7D8F5BDC}"/>
-    <hyperlink ref="F9" r:id="rId4" xr:uid="{0B16819B-B6C5-B443-83E4-E64E7575DBC5}"/>
-    <hyperlink ref="G3" r:id="rId5" xr:uid="{9E64481A-21B7-FA40-B839-4527BAD6F368}"/>
-    <hyperlink ref="F11" r:id="rId6" xr:uid="{FBA39D92-E9B8-B947-807D-B92B1457E13D}"/>
-    <hyperlink ref="F15" r:id="rId7" xr:uid="{CDC9A383-0E44-8744-9D39-55354FD83AA5}"/>
-    <hyperlink ref="F4" r:id="rId8" xr:uid="{F9D7AFCB-4795-3647-9ED8-EB4EF101C7E7}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAC86840-D8AD-F542-98B2-FC57B25AE1B6}">
-  <dimension ref="A1:L21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <cols>
-    <col min="1" max="16384" width="10.83203125" style="74"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12">
-      <c r="A1" s="74" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="74" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="74" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="74" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="74" t="s">
-        <v>78</v>
-      </c>
-      <c r="F1" s="74" t="s">
-        <v>119</v>
-      </c>
-      <c r="G1" s="74" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="74" t="s">
-        <v>267</v>
-      </c>
-      <c r="J1" s="74" t="s">
-        <v>271</v>
-      </c>
-      <c r="K1" s="74" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12">
-      <c r="A2" s="83" t="s">
-        <v>243</v>
-      </c>
-      <c r="B2" s="83" t="s">
-        <v>269</v>
-      </c>
-      <c r="C2" s="83"/>
-      <c r="D2" s="83" t="s">
-        <v>268</v>
-      </c>
-      <c r="E2" s="83"/>
-      <c r="F2" s="83"/>
-      <c r="G2" s="83"/>
-      <c r="H2" s="83" t="s">
-        <v>276</v>
-      </c>
-      <c r="I2" s="83" t="s">
-        <v>270</v>
-      </c>
-      <c r="J2" s="83" t="s">
-        <v>277</v>
-      </c>
-      <c r="K2" s="84"/>
-      <c r="L2" s="80"/>
-    </row>
-    <row r="3" spans="1:12">
-      <c r="A3" s="80" t="s">
-        <v>244</v>
-      </c>
-      <c r="B3" s="81" t="s">
-        <v>273</v>
-      </c>
-      <c r="C3" s="80"/>
-      <c r="D3" s="80"/>
-      <c r="E3" s="80"/>
-      <c r="F3" s="80" t="s">
-        <v>272</v>
-      </c>
-      <c r="G3" s="82" t="s">
-        <v>274</v>
-      </c>
-      <c r="H3" s="80" t="s">
-        <v>252</v>
-      </c>
-      <c r="I3" s="80"/>
-      <c r="J3" s="80"/>
-      <c r="K3" s="80"/>
-      <c r="L3" s="80"/>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="A4" s="83" t="s">
-        <v>136</v>
-      </c>
-      <c r="B4" s="83" t="s">
-        <v>245</v>
-      </c>
-      <c r="C4" s="83">
-        <v>1</v>
-      </c>
-      <c r="D4" s="83"/>
-      <c r="E4" s="83"/>
-      <c r="F4" s="83" t="s">
-        <v>258</v>
-      </c>
-      <c r="G4" s="86" t="s">
-        <v>275</v>
-      </c>
-      <c r="H4" s="83" t="s">
-        <v>255</v>
-      </c>
-      <c r="I4" s="80" t="s">
-        <v>259</v>
-      </c>
-      <c r="J4" s="80"/>
-      <c r="K4" s="85"/>
-      <c r="L4" s="80"/>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="A5" s="77" t="s">
-        <v>246</v>
-      </c>
-      <c r="B5" s="77"/>
-      <c r="C5" s="77"/>
-      <c r="D5" s="77"/>
-      <c r="E5" s="77"/>
-      <c r="F5" s="77"/>
-      <c r="G5" s="77"/>
-      <c r="H5" s="77" t="s">
-        <v>257</v>
-      </c>
-      <c r="J5" s="74" t="s">
-        <v>281</v>
-      </c>
-      <c r="K5" s="79"/>
-      <c r="L5" s="74" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6" s="74" t="s">
-        <v>251</v>
-      </c>
-      <c r="B6" s="75" t="s">
-        <v>247</v>
-      </c>
-      <c r="F6" s="74" t="s">
-        <v>260</v>
-      </c>
-      <c r="G6" s="74" t="s">
-        <v>261</v>
-      </c>
-      <c r="H6" s="74" t="s">
-        <v>253</v>
-      </c>
-      <c r="J6" s="74" t="s">
-        <v>263</v>
-      </c>
-      <c r="K6" s="78"/>
-      <c r="L6" s="87" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="A7" s="74" t="s">
-        <v>248</v>
-      </c>
-      <c r="B7" s="74" t="s">
-        <v>249</v>
-      </c>
-      <c r="F7" s="74" t="s">
-        <v>262</v>
-      </c>
-      <c r="G7" s="76" t="s">
-        <v>266</v>
-      </c>
-      <c r="H7" s="74" t="s">
-        <v>256</v>
-      </c>
-      <c r="K7" s="78"/>
-      <c r="L7" s="87" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="B8" s="80" t="s">
-        <v>264</v>
-      </c>
-      <c r="C8" s="80"/>
-      <c r="D8" s="80" t="s">
-        <v>250</v>
-      </c>
-      <c r="E8" s="80"/>
-      <c r="F8" s="80" t="s">
-        <v>265</v>
-      </c>
-      <c r="G8" s="82" t="s">
-        <v>261</v>
-      </c>
-      <c r="H8" s="80" t="s">
-        <v>254</v>
-      </c>
-      <c r="I8" s="80"/>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="J11" s="74" t="s">
-        <v>284</v>
-      </c>
-      <c r="K11" s="88" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="19">
-      <c r="A12" s="74" t="s">
-        <v>195</v>
-      </c>
-      <c r="K12" s="89" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="19">
-      <c r="A13" s="74" t="s">
-        <v>196</v>
-      </c>
-      <c r="K13" s="90" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
-      <c r="J14" s="74" t="s">
-        <v>286</v>
-      </c>
-      <c r="K14" s="91" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12">
-      <c r="J15" s="92" t="s">
-        <v>288</v>
-      </c>
-      <c r="K15" s="74" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
-      <c r="J16" s="74" t="s">
-        <v>290</v>
-      </c>
-      <c r="K16" s="92" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="17" spans="10:11">
-      <c r="J17" s="74" t="s">
-        <v>291</v>
-      </c>
-      <c r="K17" s="91" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="18" spans="10:11">
-      <c r="J18" s="74" t="s">
-        <v>293</v>
-      </c>
-      <c r="K18" s="91" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="19" spans="10:11">
-      <c r="J19" s="74" t="s">
-        <v>295</v>
-      </c>
-      <c r="K19" s="91" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="20" spans="10:11">
-      <c r="J20" s="74" t="s">
-        <v>299</v>
-      </c>
-      <c r="K20" s="74" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="21" spans="10:11">
-      <c r="K21" s="74" t="s">
-        <v>301</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB09F318-339D-2C4D-BE3F-E973DAF25A4A}">
   <dimension ref="A1:R41"/>
   <sheetViews>
@@ -4962,1168 +6325,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E531EC0F-8B5B-B945-81ED-74853B083270}">
-  <dimension ref="A1:R41"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J27" sqref="A1:J27"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
-  <cols>
-    <col min="1" max="5" width="10.83203125" style="1"/>
-    <col min="6" max="6" width="26.6640625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:18">
-      <c r="I1" s="9"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
-      <c r="Q1" s="30"/>
-      <c r="R1" s="30"/>
-    </row>
-    <row r="2" spans="1:18">
-      <c r="A2" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="I2" s="9"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="30"/>
-      <c r="Q2" s="30"/>
-      <c r="R2" s="30"/>
-    </row>
-    <row r="3" spans="1:18">
-      <c r="A3" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="30" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="30" t="s">
-        <v>78</v>
-      </c>
-      <c r="F3" s="30" t="s">
-        <v>119</v>
-      </c>
-      <c r="G3" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" s="30"/>
-      <c r="I3" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="J3" s="7"/>
-      <c r="K3" s="30"/>
-      <c r="L3" s="30"/>
-      <c r="M3" s="30"/>
-      <c r="N3" s="30"/>
-      <c r="O3" s="30"/>
-      <c r="P3" s="30"/>
-      <c r="Q3" s="30"/>
-      <c r="R3" s="30"/>
-    </row>
-    <row r="4" spans="1:18">
-      <c r="A4" s="44" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="44">
-        <v>1</v>
-      </c>
-      <c r="D4" s="44" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="49" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="7">
-        <v>560</v>
-      </c>
-      <c r="J4" s="7"/>
-      <c r="K4" s="30"/>
-      <c r="L4" s="30"/>
-      <c r="M4" s="30"/>
-      <c r="N4" s="30"/>
-      <c r="O4" s="30"/>
-      <c r="P4" s="30"/>
-      <c r="Q4" s="30"/>
-      <c r="R4" s="30"/>
-    </row>
-    <row r="5" spans="1:18">
-      <c r="A5" s="30" t="s">
-        <v>97</v>
-      </c>
-      <c r="B5" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="30">
-        <v>5</v>
-      </c>
-      <c r="D5" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" s="30"/>
-      <c r="I5" s="7">
-        <v>452000</v>
-      </c>
-      <c r="J5" s="7"/>
-      <c r="K5" s="30"/>
-      <c r="L5" s="30"/>
-      <c r="M5" s="30"/>
-      <c r="N5" s="30"/>
-      <c r="O5" s="30"/>
-      <c r="P5" s="30"/>
-      <c r="Q5" s="30"/>
-      <c r="R5" s="30"/>
-    </row>
-    <row r="6" spans="1:18">
-      <c r="A6" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="30">
-        <v>1</v>
-      </c>
-      <c r="D6" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" s="36"/>
-      <c r="H6" s="36"/>
-      <c r="I6" s="7">
-        <v>2500</v>
-      </c>
-      <c r="J6" s="7"/>
-      <c r="K6" s="22"/>
-      <c r="L6" s="30"/>
-      <c r="M6" s="30"/>
-      <c r="N6" s="30"/>
-      <c r="O6" s="30"/>
-      <c r="P6" s="30"/>
-      <c r="Q6" s="30"/>
-      <c r="R6" s="30"/>
-    </row>
-    <row r="7" spans="1:18">
-      <c r="A7" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="30">
-        <v>1</v>
-      </c>
-      <c r="D7" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="H7" s="30"/>
-      <c r="I7" s="7">
-        <v>49000</v>
-      </c>
-      <c r="J7" s="7"/>
-      <c r="K7" s="30"/>
-      <c r="L7" s="30"/>
-      <c r="M7" s="30"/>
-      <c r="N7" s="30"/>
-      <c r="O7" s="30"/>
-      <c r="P7" s="30"/>
-      <c r="Q7" s="30"/>
-      <c r="R7" s="30"/>
-    </row>
-    <row r="8" spans="1:18">
-      <c r="A8" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="C8" s="30">
-        <v>1</v>
-      </c>
-      <c r="D8" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="30" t="s">
-        <v>81</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="G8" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="H8" s="30"/>
-      <c r="I8" s="7">
-        <v>684</v>
-      </c>
-      <c r="J8" s="7"/>
-      <c r="K8" s="30"/>
-      <c r="L8" s="30"/>
-      <c r="M8" s="30"/>
-      <c r="N8" s="30"/>
-      <c r="O8" s="30"/>
-      <c r="P8" s="30"/>
-      <c r="Q8" s="30"/>
-      <c r="R8" s="30"/>
-    </row>
-    <row r="9" spans="1:18">
-      <c r="A9" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="B9" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="30">
-        <v>2</v>
-      </c>
-      <c r="D9" s="30" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="36" t="s">
-        <v>112</v>
-      </c>
-      <c r="G9" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="H9" s="30"/>
-      <c r="I9" s="7">
-        <v>17500</v>
-      </c>
-      <c r="J9" s="7"/>
-      <c r="K9" s="30"/>
-      <c r="L9" s="30"/>
-      <c r="M9" s="30"/>
-      <c r="N9" s="30"/>
-      <c r="O9" s="30"/>
-      <c r="P9" s="30"/>
-      <c r="Q9" s="30"/>
-      <c r="R9" s="30"/>
-    </row>
-    <row r="10" spans="1:18">
-      <c r="A10" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="30">
-        <v>5</v>
-      </c>
-      <c r="D10" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="7">
-        <v>42000</v>
-      </c>
-      <c r="J10" s="7"/>
-      <c r="K10" s="30"/>
-      <c r="L10" s="30"/>
-      <c r="M10" s="30"/>
-      <c r="N10" s="30"/>
-      <c r="O10" s="30"/>
-      <c r="P10" s="30"/>
-      <c r="Q10" s="30"/>
-      <c r="R10" s="30"/>
-    </row>
-    <row r="11" spans="1:18">
-      <c r="A11" s="30" t="s">
-        <v>95</v>
-      </c>
-      <c r="B11" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="C11" s="30">
-        <v>7</v>
-      </c>
-      <c r="D11" s="30" t="s">
-        <v>43</v>
-      </c>
-      <c r="E11" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="G11" s="36"/>
-      <c r="H11" s="30" t="s">
-        <v>90</v>
-      </c>
-      <c r="I11" s="7">
-        <v>75000</v>
-      </c>
-      <c r="J11" s="7"/>
-      <c r="K11" s="30"/>
-      <c r="L11" s="30"/>
-      <c r="M11" s="30"/>
-      <c r="N11" s="30"/>
-      <c r="O11" s="30"/>
-      <c r="P11" s="30"/>
-      <c r="Q11" s="30"/>
-      <c r="R11" s="30"/>
-    </row>
-    <row r="12" spans="1:18">
-      <c r="A12" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="B12" s="37" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="30">
-        <v>3</v>
-      </c>
-      <c r="D12" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="E12" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="G12" s="36"/>
-      <c r="H12" s="30" t="s">
-        <v>90</v>
-      </c>
-      <c r="I12" s="7">
-        <v>283000</v>
-      </c>
-      <c r="J12" s="7"/>
-      <c r="K12" s="30"/>
-      <c r="L12" s="30"/>
-      <c r="M12" s="30"/>
-      <c r="N12" s="30"/>
-      <c r="O12" s="30"/>
-      <c r="P12" s="30"/>
-      <c r="Q12" s="30"/>
-      <c r="R12" s="30"/>
-    </row>
-    <row r="13" spans="1:18">
-      <c r="A13" s="30" t="s">
-        <v>100</v>
-      </c>
-      <c r="B13" s="30" t="s">
-        <v>98</v>
-      </c>
-      <c r="C13" s="30">
-        <v>4</v>
-      </c>
-      <c r="D13" s="37">
-        <v>82</v>
-      </c>
-      <c r="E13" s="30" t="s">
-        <v>98</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="G13" s="36"/>
-      <c r="H13" s="36"/>
-      <c r="I13" s="7">
-        <v>100000</v>
-      </c>
-      <c r="J13" s="7"/>
-      <c r="K13" s="30"/>
-      <c r="L13" s="30"/>
-      <c r="M13" s="30"/>
-      <c r="N13" s="30"/>
-      <c r="O13" s="30"/>
-      <c r="P13" s="30"/>
-      <c r="Q13" s="30"/>
-      <c r="R13" s="30"/>
-    </row>
-    <row r="14" spans="1:18">
-      <c r="A14" s="30"/>
-      <c r="B14" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="C14" s="30">
-        <v>24</v>
-      </c>
-      <c r="D14" s="37" t="s">
-        <v>47</v>
-      </c>
-      <c r="E14" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="G14" s="30" t="s">
-        <v>50</v>
-      </c>
-      <c r="H14" s="30"/>
-      <c r="I14" s="7">
-        <v>20390000</v>
-      </c>
-      <c r="J14" s="7"/>
-      <c r="K14" s="30"/>
-      <c r="L14" s="30"/>
-      <c r="M14" s="30"/>
-      <c r="N14" s="30"/>
-      <c r="O14" s="30"/>
-      <c r="P14" s="30"/>
-      <c r="Q14" s="30"/>
-      <c r="R14" s="30"/>
-    </row>
-    <row r="15" spans="1:18">
-      <c r="A15" s="30" t="s">
-        <v>102</v>
-      </c>
-      <c r="B15" s="30" t="s">
-        <v>91</v>
-      </c>
-      <c r="C15" s="30">
-        <v>1</v>
-      </c>
-      <c r="D15" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="E15" s="30" t="s">
-        <v>92</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="H15" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="I15" s="7">
-        <v>4000</v>
-      </c>
-      <c r="J15" s="7"/>
-      <c r="K15" s="30"/>
-      <c r="L15" s="30"/>
-      <c r="M15" s="30"/>
-      <c r="N15" s="30"/>
-      <c r="O15" s="30"/>
-      <c r="P15" s="30"/>
-      <c r="Q15" s="30"/>
-      <c r="R15" s="30"/>
-    </row>
-    <row r="16" spans="1:18">
-      <c r="A16" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="B16" s="30" t="s">
-        <v>87</v>
-      </c>
-      <c r="C16" s="30">
-        <v>1</v>
-      </c>
-      <c r="D16" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="E16" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="G16" s="36"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="7">
-        <v>4500</v>
-      </c>
-      <c r="J16" s="7"/>
-      <c r="K16" s="30"/>
-      <c r="L16" s="30"/>
-      <c r="M16" s="30"/>
-      <c r="N16" s="30"/>
-      <c r="O16" s="18"/>
-      <c r="P16" s="30" t="s">
-        <v>144</v>
-      </c>
-      <c r="Q16" s="30"/>
-      <c r="R16" s="30" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18">
-      <c r="A17" s="40" t="s">
-        <v>136</v>
-      </c>
-      <c r="B17" s="41" t="s">
-        <v>150</v>
-      </c>
-      <c r="C17" s="40">
-        <v>1</v>
-      </c>
-      <c r="D17" s="40" t="s">
-        <v>54</v>
-      </c>
-      <c r="E17" s="42" t="s">
-        <v>130</v>
-      </c>
-      <c r="F17" s="50" t="s">
-        <v>156</v>
-      </c>
-      <c r="G17" s="51"/>
-      <c r="H17" s="43" t="s">
-        <v>157</v>
-      </c>
-      <c r="I17" s="52">
-        <v>2</v>
-      </c>
-      <c r="J17" s="7"/>
-      <c r="K17" s="30"/>
-      <c r="L17" s="30"/>
-      <c r="M17" s="30"/>
-      <c r="N17" s="30"/>
-      <c r="O17" s="29"/>
-      <c r="P17" s="30" t="s">
-        <v>148</v>
-      </c>
-      <c r="Q17" s="30" t="s">
-        <v>147</v>
-      </c>
-      <c r="R17" s="30"/>
-    </row>
-    <row r="18" spans="1:18">
-      <c r="A18" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="B18" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="C18" s="39" t="s">
-        <v>125</v>
-      </c>
-      <c r="D18" s="30" t="s">
-        <v>69</v>
-      </c>
-      <c r="E18" s="25" t="s">
-        <v>130</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="G18" s="36"/>
-      <c r="H18" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="30"/>
-      <c r="L18" s="30"/>
-      <c r="M18" s="30"/>
-      <c r="N18" s="30"/>
-      <c r="O18" s="18"/>
-      <c r="P18" s="30" t="s">
-        <v>151</v>
-      </c>
-      <c r="Q18" s="30" t="s">
-        <v>152</v>
-      </c>
-      <c r="R18" s="30"/>
-    </row>
-    <row r="19" spans="1:18">
-      <c r="A19" s="38" t="s">
-        <v>113</v>
-      </c>
-      <c r="B19" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="C19" s="30"/>
-      <c r="D19" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="E19" s="30" t="s">
-        <v>77</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="G19" s="36"/>
-      <c r="H19" s="36"/>
-      <c r="I19" s="7">
-        <v>60</v>
-      </c>
-      <c r="J19" s="7"/>
-      <c r="K19" s="30"/>
-      <c r="L19" s="30"/>
-      <c r="M19" s="30"/>
-      <c r="N19" s="30"/>
-      <c r="O19" s="18"/>
-      <c r="P19" s="30" t="s">
-        <v>154</v>
-      </c>
-      <c r="Q19" s="30" t="s">
-        <v>153</v>
-      </c>
-      <c r="R19" s="30"/>
-    </row>
-    <row r="20" spans="1:18">
-      <c r="A20" s="38" t="s">
-        <v>132</v>
-      </c>
-      <c r="B20" s="25" t="s">
-        <v>104</v>
-      </c>
-      <c r="C20" s="30">
-        <v>1</v>
-      </c>
-      <c r="D20" s="30" t="s">
-        <v>105</v>
-      </c>
-      <c r="E20" s="25" t="s">
-        <v>104</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="G20" s="30"/>
-      <c r="H20" s="30"/>
-      <c r="I20" s="23">
-        <v>758</v>
-      </c>
-      <c r="J20" s="7"/>
-      <c r="K20" s="22"/>
-      <c r="L20" s="30"/>
-      <c r="M20" s="30"/>
-      <c r="N20" s="30"/>
-      <c r="O20" s="30"/>
-      <c r="P20" s="30"/>
-      <c r="Q20" s="30"/>
-      <c r="R20" s="30"/>
-    </row>
-    <row r="21" spans="1:18">
-      <c r="A21" s="30" t="s">
-        <v>133</v>
-      </c>
-      <c r="B21" s="30" t="s">
-        <v>56</v>
-      </c>
-      <c r="C21" s="30">
-        <v>1</v>
-      </c>
-      <c r="D21" s="30" t="s">
-        <v>101</v>
-      </c>
-      <c r="E21" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="G21" s="36"/>
-      <c r="H21" s="36"/>
-      <c r="I21" s="7">
-        <v>35000</v>
-      </c>
-      <c r="J21" s="7"/>
-      <c r="K21" s="30"/>
-      <c r="L21" s="30"/>
-      <c r="M21" s="30"/>
-      <c r="N21" s="30"/>
-      <c r="O21" s="30"/>
-      <c r="P21" s="30"/>
-      <c r="Q21" s="30"/>
-      <c r="R21" s="30"/>
-    </row>
-    <row r="22" spans="1:18">
-      <c r="A22" s="30" t="s">
-        <v>134</v>
-      </c>
-      <c r="B22" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="C22" s="30">
-        <v>1</v>
-      </c>
-      <c r="D22" s="30" t="s">
-        <v>86</v>
-      </c>
-      <c r="E22" s="30" t="s">
-        <v>85</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="G22" s="36"/>
-      <c r="H22" s="36"/>
-      <c r="I22" s="7">
-        <v>7500</v>
-      </c>
-      <c r="J22" s="7"/>
-      <c r="K22" s="30"/>
-      <c r="L22" s="30"/>
-      <c r="M22" s="30"/>
-      <c r="N22" s="30"/>
-      <c r="O22" s="30"/>
-      <c r="P22" s="30"/>
-      <c r="Q22" s="30"/>
-      <c r="R22" s="30"/>
-    </row>
-    <row r="23" spans="1:18">
-      <c r="A23" s="44" t="s">
-        <v>67</v>
-      </c>
-      <c r="B23" s="41" t="s">
-        <v>107</v>
-      </c>
-      <c r="C23" s="44">
-        <v>1</v>
-      </c>
-      <c r="D23" s="46" t="s">
-        <v>108</v>
-      </c>
-      <c r="E23" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="F23" s="49" t="s">
-        <v>122</v>
-      </c>
-      <c r="G23" s="45"/>
-      <c r="H23" s="44" t="s">
-        <v>139</v>
-      </c>
-      <c r="I23" s="7">
-        <v>15000</v>
-      </c>
-      <c r="J23" s="9"/>
-      <c r="M23" s="30"/>
-      <c r="N23" s="30"/>
-      <c r="O23" s="30"/>
-      <c r="P23" s="30"/>
-      <c r="Q23" s="30"/>
-      <c r="R23" s="30"/>
-    </row>
-    <row r="24" spans="1:18">
-      <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="30"/>
-      <c r="L24" s="30"/>
-      <c r="M24" s="30"/>
-      <c r="N24" s="30"/>
-      <c r="O24" s="30"/>
-      <c r="P24" s="30"/>
-      <c r="Q24" s="30"/>
-      <c r="R24" s="30"/>
-    </row>
-    <row r="25" spans="1:18">
-      <c r="A25" s="30" t="s">
-        <v>159</v>
-      </c>
-      <c r="B25" s="20"/>
-      <c r="C25" s="30"/>
-      <c r="D25" s="30"/>
-      <c r="E25" s="30"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="30"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="7"/>
-      <c r="J25" s="7"/>
-      <c r="K25" s="30"/>
-      <c r="L25" s="30"/>
-      <c r="M25" s="30"/>
-      <c r="N25" s="30"/>
-      <c r="O25" s="30"/>
-      <c r="P25" s="30"/>
-      <c r="Q25" s="30"/>
-      <c r="R25" s="30"/>
-    </row>
-    <row r="26" spans="1:18">
-      <c r="A26" s="48" t="s">
-        <v>138</v>
-      </c>
-      <c r="B26" s="48" t="s">
-        <v>141</v>
-      </c>
-      <c r="C26" s="48">
-        <v>1</v>
-      </c>
-      <c r="D26" s="48" t="s">
-        <v>140</v>
-      </c>
-      <c r="E26" s="48"/>
-      <c r="F26" s="49" t="s">
-        <v>146</v>
-      </c>
-      <c r="G26" s="48"/>
-      <c r="H26" s="48"/>
-      <c r="I26" s="9"/>
-      <c r="J26" s="7"/>
-      <c r="K26" s="30"/>
-      <c r="L26" s="30"/>
-      <c r="M26" s="30"/>
-      <c r="N26" s="30"/>
-      <c r="O26" s="30"/>
-      <c r="P26" s="30"/>
-      <c r="Q26" s="30"/>
-      <c r="R26" s="30"/>
-    </row>
-    <row r="27" spans="1:18">
-      <c r="I27" s="9"/>
-      <c r="J27" s="7"/>
-      <c r="K27" s="30"/>
-      <c r="L27" s="30"/>
-      <c r="M27" s="30"/>
-      <c r="N27" s="30"/>
-      <c r="O27" s="30"/>
-      <c r="P27" s="30"/>
-      <c r="Q27" s="30"/>
-      <c r="R27" s="30"/>
-    </row>
-    <row r="28" spans="1:18">
-      <c r="I28" s="9"/>
-      <c r="J28" s="9"/>
-      <c r="L28" s="30"/>
-      <c r="M28" s="30"/>
-      <c r="N28" s="30"/>
-      <c r="O28" s="30"/>
-      <c r="P28" s="30"/>
-      <c r="Q28" s="30"/>
-      <c r="R28" s="30"/>
-    </row>
-    <row r="29" spans="1:18">
-      <c r="A29" s="30"/>
-      <c r="B29" s="30"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="30"/>
-      <c r="G29" s="30"/>
-      <c r="H29" s="30"/>
-      <c r="I29" s="30"/>
-      <c r="J29" s="30"/>
-      <c r="K29" s="30"/>
-      <c r="L29" s="30"/>
-      <c r="M29" s="30"/>
-      <c r="N29" s="30"/>
-      <c r="O29" s="30"/>
-      <c r="P29" s="30"/>
-      <c r="Q29" s="30"/>
-      <c r="R29" s="30"/>
-    </row>
-    <row r="30" spans="1:18">
-      <c r="A30" s="30"/>
-      <c r="B30" s="30"/>
-      <c r="C30" s="30"/>
-      <c r="D30" s="30"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="30"/>
-      <c r="G30" s="30"/>
-      <c r="H30" s="30"/>
-      <c r="I30" s="30"/>
-      <c r="J30" s="30"/>
-      <c r="K30" s="30"/>
-      <c r="L30" s="30"/>
-      <c r="M30" s="30"/>
-      <c r="N30" s="30"/>
-      <c r="O30" s="30"/>
-      <c r="P30" s="30"/>
-      <c r="Q30" s="30"/>
-      <c r="R30" s="30"/>
-    </row>
-    <row r="31" spans="1:18">
-      <c r="A31" s="30"/>
-      <c r="B31" s="30"/>
-      <c r="C31" s="30"/>
-      <c r="D31" s="30"/>
-      <c r="E31" s="30"/>
-      <c r="F31" s="30"/>
-      <c r="G31" s="30"/>
-      <c r="H31" s="30"/>
-      <c r="I31" s="30"/>
-      <c r="J31" s="30"/>
-      <c r="K31" s="30"/>
-      <c r="L31" s="30"/>
-      <c r="M31" s="30"/>
-      <c r="N31" s="30"/>
-      <c r="O31" s="30"/>
-      <c r="P31" s="30"/>
-      <c r="Q31" s="30"/>
-      <c r="R31" s="30"/>
-    </row>
-    <row r="32" spans="1:18">
-      <c r="A32" s="30"/>
-      <c r="B32" s="30"/>
-      <c r="C32" s="30"/>
-      <c r="D32" s="30"/>
-      <c r="E32" s="30"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="36"/>
-      <c r="H32" s="36"/>
-      <c r="I32" s="28"/>
-      <c r="J32" s="30"/>
-      <c r="K32" s="30"/>
-      <c r="L32" s="30"/>
-      <c r="M32" s="30"/>
-      <c r="N32" s="30"/>
-      <c r="O32" s="30"/>
-      <c r="P32" s="30"/>
-      <c r="Q32" s="30"/>
-      <c r="R32" s="30"/>
-    </row>
-    <row r="33" spans="1:18">
-      <c r="A33" s="30"/>
-      <c r="B33" s="18"/>
-      <c r="C33" s="30"/>
-      <c r="D33" s="30"/>
-      <c r="E33" s="30"/>
-      <c r="F33" s="30"/>
-      <c r="G33" s="30"/>
-      <c r="H33" s="30"/>
-      <c r="I33" s="30"/>
-      <c r="J33" s="30"/>
-      <c r="K33" s="30"/>
-      <c r="L33" s="30"/>
-      <c r="M33" s="30"/>
-      <c r="N33" s="30"/>
-      <c r="O33" s="30"/>
-      <c r="P33" s="30"/>
-      <c r="Q33" s="30"/>
-      <c r="R33" s="30"/>
-    </row>
-    <row r="34" spans="1:18">
-      <c r="A34" s="30"/>
-      <c r="B34" s="29"/>
-      <c r="C34" s="30"/>
-      <c r="D34" s="30"/>
-      <c r="E34" s="30"/>
-      <c r="F34" s="30"/>
-      <c r="G34" s="30"/>
-      <c r="H34" s="30"/>
-      <c r="I34" s="30"/>
-      <c r="J34" s="30"/>
-      <c r="K34" s="30"/>
-      <c r="L34" s="30"/>
-      <c r="M34" s="30"/>
-      <c r="N34" s="30"/>
-      <c r="O34" s="30"/>
-      <c r="P34" s="30"/>
-      <c r="Q34" s="30"/>
-      <c r="R34" s="30"/>
-    </row>
-    <row r="35" spans="1:18">
-      <c r="A35" s="30"/>
-      <c r="B35" s="18"/>
-      <c r="C35" s="30"/>
-      <c r="D35" s="30"/>
-      <c r="E35" s="30"/>
-      <c r="F35" s="30"/>
-      <c r="G35" s="30"/>
-      <c r="H35" s="30"/>
-      <c r="I35" s="30"/>
-      <c r="J35" s="30"/>
-      <c r="K35" s="30"/>
-      <c r="L35" s="30"/>
-      <c r="M35" s="30"/>
-      <c r="N35" s="30"/>
-      <c r="O35" s="30"/>
-      <c r="P35" s="30"/>
-      <c r="Q35" s="30"/>
-      <c r="R35" s="30"/>
-    </row>
-    <row r="36" spans="1:18">
-      <c r="A36" s="30"/>
-      <c r="B36" s="18"/>
-      <c r="C36" s="30"/>
-      <c r="D36" s="30"/>
-      <c r="E36" s="30"/>
-      <c r="F36" s="30"/>
-      <c r="G36" s="30"/>
-      <c r="H36" s="30"/>
-      <c r="I36" s="30"/>
-      <c r="J36" s="30"/>
-      <c r="K36" s="30"/>
-      <c r="L36" s="30"/>
-      <c r="M36" s="30"/>
-      <c r="N36" s="30"/>
-      <c r="O36" s="30"/>
-      <c r="P36" s="30"/>
-      <c r="Q36" s="30"/>
-      <c r="R36" s="30"/>
-    </row>
-    <row r="37" spans="1:18">
-      <c r="A37" s="30"/>
-      <c r="B37" s="30"/>
-      <c r="C37" s="30"/>
-      <c r="D37" s="30"/>
-      <c r="E37" s="30"/>
-      <c r="F37" s="30"/>
-      <c r="G37" s="30"/>
-      <c r="H37" s="30"/>
-      <c r="I37" s="30"/>
-      <c r="J37" s="30"/>
-      <c r="K37" s="30"/>
-      <c r="L37" s="30"/>
-      <c r="M37" s="30"/>
-      <c r="N37" s="30"/>
-      <c r="O37" s="30"/>
-      <c r="P37" s="30"/>
-      <c r="Q37" s="30"/>
-      <c r="R37" s="30"/>
-    </row>
-    <row r="38" spans="1:18">
-      <c r="A38" s="30"/>
-      <c r="B38" s="30"/>
-      <c r="C38" s="30"/>
-      <c r="D38" s="30"/>
-      <c r="E38" s="30"/>
-      <c r="F38" s="30"/>
-      <c r="G38" s="30"/>
-      <c r="H38" s="30"/>
-      <c r="I38" s="30"/>
-      <c r="J38" s="30"/>
-      <c r="K38" s="30"/>
-      <c r="L38" s="30"/>
-      <c r="M38" s="30"/>
-      <c r="N38" s="30"/>
-      <c r="O38" s="30"/>
-      <c r="P38" s="30"/>
-      <c r="Q38" s="30"/>
-      <c r="R38" s="30"/>
-    </row>
-    <row r="39" spans="1:18">
-      <c r="A39" s="30"/>
-      <c r="B39" s="30"/>
-      <c r="C39" s="30"/>
-      <c r="D39" s="30"/>
-      <c r="E39" s="30"/>
-      <c r="F39" s="30"/>
-      <c r="G39" s="30"/>
-      <c r="H39" s="30"/>
-      <c r="I39" s="30"/>
-      <c r="J39" s="30"/>
-      <c r="K39" s="30"/>
-      <c r="L39" s="30"/>
-      <c r="M39" s="30"/>
-      <c r="N39" s="30"/>
-      <c r="O39" s="30"/>
-      <c r="P39" s="30"/>
-      <c r="Q39" s="30"/>
-      <c r="R39" s="30"/>
-    </row>
-    <row r="40" spans="1:18">
-      <c r="A40" s="30"/>
-      <c r="B40" s="30"/>
-      <c r="C40" s="30"/>
-      <c r="D40" s="30"/>
-      <c r="E40" s="30"/>
-      <c r="F40" s="30"/>
-      <c r="G40" s="30"/>
-      <c r="H40" s="30"/>
-      <c r="I40" s="30"/>
-      <c r="J40" s="30"/>
-      <c r="K40" s="30"/>
-      <c r="L40" s="30"/>
-      <c r="M40" s="30"/>
-      <c r="N40" s="30"/>
-      <c r="O40" s="30"/>
-      <c r="P40" s="30"/>
-      <c r="Q40" s="30"/>
-      <c r="R40" s="30"/>
-    </row>
-    <row r="41" spans="1:18">
-      <c r="A41" s="30"/>
-      <c r="B41" s="37"/>
-      <c r="C41" s="30"/>
-      <c r="D41" s="30"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="6"/>
-      <c r="G41" s="36"/>
-      <c r="H41" s="36"/>
-      <c r="I41" s="30"/>
-      <c r="J41" s="30"/>
-      <c r="K41" s="30"/>
-      <c r="L41" s="30"/>
-      <c r="M41" s="30"/>
-      <c r="N41" s="30"/>
-      <c r="O41" s="30"/>
-      <c r="P41" s="30"/>
-      <c r="Q41" s="30"/>
-      <c r="R41" s="30"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="F4" r:id="rId1" xr:uid="{8D1A619E-9515-524F-B85A-A336184FAF79}"/>
-    <hyperlink ref="F5" r:id="rId2" xr:uid="{3AAC0776-E199-2D4D-A06E-B69343AE631B}"/>
-    <hyperlink ref="F6" r:id="rId3" xr:uid="{E461B325-C0F0-DA45-BDA8-84250934722A}"/>
-    <hyperlink ref="F7" r:id="rId4" xr:uid="{A60C7027-4B10-1E42-84BA-150AC300C862}"/>
-    <hyperlink ref="F8" r:id="rId5" xr:uid="{A1B92DA8-9C86-894C-993F-E8279B7DC277}"/>
-    <hyperlink ref="F10" r:id="rId6" xr:uid="{2515C9A8-0A71-A542-9DE7-C8FE503FC70A}"/>
-    <hyperlink ref="F11" r:id="rId7" display="https://www.digikey.com/product-detail/en/vishay-siliconix/2N7002E-T1-E3/2N7002E-T1-E3CT-ND/3946142?utm_adgroup=Semiconductor%20Modules&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Dynamic%20Search_RLSA_Buyers&amp;utm_term=&amp;utm_content=Semiconductor%20Modules&amp;gclid=Cj0KCQjwrIf3BRD1ARIsAMuugNtAYg0B4uzN6uG3FDVYlywiEKFAGbXRLO8hnfXG_d9twvCOg1_5j4waAs4CEALw_wcB" xr:uid="{E2ADDD7B-C275-A94E-8AEE-3CE4B10DEC4C}"/>
-    <hyperlink ref="F12" r:id="rId8" xr:uid="{27125482-B106-0147-B5B6-DE477125A0DC}"/>
-    <hyperlink ref="F13" r:id="rId9" xr:uid="{4CA4B337-CA91-E94E-B1F9-390ABAD5A837}"/>
-    <hyperlink ref="F14" r:id="rId10" xr:uid="{C48CA423-8ACC-8844-A5D3-14CB3B73FE20}"/>
-    <hyperlink ref="F15" r:id="rId11" xr:uid="{09C32FBB-C794-C744-A726-DDD0502B59F8}"/>
-    <hyperlink ref="F16" r:id="rId12" xr:uid="{C74B4AAC-4139-E74C-AA5B-14D06E76C48A}"/>
-    <hyperlink ref="F17" r:id="rId13" display="https://www.digikey.com/product-detail/en/inspired-led-llc/12V-SB-RGB-5M/1647-1069-2-ND/9091794" xr:uid="{BE2E3CAA-1537-B94B-BB1B-68FD97458555}"/>
-    <hyperlink ref="F18" r:id="rId14" xr:uid="{FD5CF46B-0193-D147-9826-48512F9DED48}"/>
-    <hyperlink ref="F19" r:id="rId15" xr:uid="{B100B64A-F971-F14A-ADEA-BBCFCD09A1AA}"/>
-    <hyperlink ref="F20" r:id="rId16" display="https://www.digikey.com/products/en?keywords=1658623-3" xr:uid="{1726C16B-1136-D04D-BE50-29799826E622}"/>
-    <hyperlink ref="F21" r:id="rId17" xr:uid="{646AFD14-92B1-D340-840C-800535B95EDE}"/>
-    <hyperlink ref="F22" r:id="rId18" xr:uid="{6AB34C14-18FE-564D-AEBF-20FEAB9DBCA9}"/>
-    <hyperlink ref="F23" r:id="rId19" display="https://www.digikey.com/product-detail/en/soberton-inc/SP-1504/433-1106-ND/3973690" xr:uid="{53C14038-FF08-BA49-8774-52E06C0F3358}"/>
-    <hyperlink ref="F26" r:id="rId20" xr:uid="{D34A9D3D-0E41-7C45-9FAE-64E42873741D}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>